<commit_message>
bugfixes in 03 and 05
</commit_message>
<xml_diff>
--- a/transformed_data/cartel_networks/cartel_df_herfindal.xlsx
+++ b/transformed_data/cartel_networks/cartel_df_herfindal.xlsx
@@ -1555,7 +1555,9 @@
       <c r="CM5" t="inlineStr"/>
       <c r="CN5" t="inlineStr"/>
       <c r="CO5" t="inlineStr"/>
-      <c r="CP5" t="inlineStr"/>
+      <c r="CP5" t="n">
+        <v>663.85</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -12800,10 +12802,18 @@
         <v>2004</v>
       </c>
       <c r="BB83" t="inlineStr"/>
-      <c r="BC83" t="inlineStr"/>
-      <c r="BD83" t="inlineStr"/>
-      <c r="BE83" t="inlineStr"/>
-      <c r="BF83" t="inlineStr"/>
+      <c r="BC83" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD83" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE83" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF83" t="n">
+        <v>0</v>
+      </c>
       <c r="BG83" t="inlineStr"/>
       <c r="BH83" t="inlineStr"/>
       <c r="BI83" t="inlineStr"/>
@@ -12836,10 +12846,18 @@
       <c r="CJ83" t="inlineStr"/>
       <c r="CK83" t="inlineStr"/>
       <c r="CL83" t="inlineStr"/>
-      <c r="CM83" t="inlineStr"/>
-      <c r="CN83" t="inlineStr"/>
-      <c r="CO83" t="inlineStr"/>
-      <c r="CP83" t="inlineStr"/>
+      <c r="CM83" t="n">
+        <v>985.9299999999999</v>
+      </c>
+      <c r="CN83" t="n">
+        <v>966.8099999999999</v>
+      </c>
+      <c r="CO83" t="n">
+        <v>964.91</v>
+      </c>
+      <c r="CP83" t="n">
+        <v>976.14</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
@@ -14998,7 +15016,9 @@
       <c r="BF98" t="inlineStr"/>
       <c r="BG98" t="inlineStr"/>
       <c r="BH98" t="inlineStr"/>
-      <c r="BI98" t="inlineStr"/>
+      <c r="BI98" t="n">
+        <v>48.8</v>
+      </c>
       <c r="BJ98" t="inlineStr"/>
       <c r="BK98" t="inlineStr"/>
       <c r="BL98" t="inlineStr"/>
@@ -15028,10 +15048,18 @@
       <c r="CJ98" t="inlineStr"/>
       <c r="CK98" t="inlineStr"/>
       <c r="CL98" t="inlineStr"/>
-      <c r="CM98" t="inlineStr"/>
-      <c r="CN98" t="inlineStr"/>
-      <c r="CO98" t="inlineStr"/>
-      <c r="CP98" t="inlineStr"/>
+      <c r="CM98" t="n">
+        <v>186.41</v>
+      </c>
+      <c r="CN98" t="n">
+        <v>196.13</v>
+      </c>
+      <c r="CO98" t="n">
+        <v>4.77</v>
+      </c>
+      <c r="CP98" t="n">
+        <v>3.52</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
@@ -17669,7 +17697,9 @@
       <c r="BO116" t="inlineStr"/>
       <c r="BP116" t="inlineStr"/>
       <c r="BQ116" t="inlineStr"/>
-      <c r="BR116" t="inlineStr"/>
+      <c r="BR116" t="n">
+        <v>48.8</v>
+      </c>
       <c r="BS116" t="inlineStr"/>
       <c r="BT116" t="inlineStr"/>
       <c r="BU116" t="inlineStr"/>
@@ -17690,10 +17720,18 @@
       <c r="CJ116" t="inlineStr"/>
       <c r="CK116" t="inlineStr"/>
       <c r="CL116" t="inlineStr"/>
-      <c r="CM116" t="inlineStr"/>
-      <c r="CN116" t="inlineStr"/>
-      <c r="CO116" t="inlineStr"/>
-      <c r="CP116" t="inlineStr"/>
+      <c r="CM116" t="n">
+        <v>186.41</v>
+      </c>
+      <c r="CN116" t="n">
+        <v>196.13</v>
+      </c>
+      <c r="CO116" t="n">
+        <v>4.77</v>
+      </c>
+      <c r="CP116" t="n">
+        <v>3.52</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
@@ -17946,10 +17984,18 @@
         <v>2004</v>
       </c>
       <c r="BB118" t="inlineStr"/>
-      <c r="BC118" t="inlineStr"/>
-      <c r="BD118" t="inlineStr"/>
-      <c r="BE118" t="inlineStr"/>
-      <c r="BF118" t="inlineStr"/>
+      <c r="BC118" t="n">
+        <v>12.94</v>
+      </c>
+      <c r="BD118" t="n">
+        <v>62.03</v>
+      </c>
+      <c r="BE118" t="n">
+        <v>80.12</v>
+      </c>
+      <c r="BF118" t="n">
+        <v>575.45</v>
+      </c>
       <c r="BG118" t="inlineStr"/>
       <c r="BH118" t="inlineStr"/>
       <c r="BI118" t="inlineStr"/>
@@ -17982,10 +18028,18 @@
       <c r="CJ118" t="inlineStr"/>
       <c r="CK118" t="inlineStr"/>
       <c r="CL118" t="inlineStr"/>
-      <c r="CM118" t="inlineStr"/>
-      <c r="CN118" t="inlineStr"/>
-      <c r="CO118" t="inlineStr"/>
-      <c r="CP118" t="inlineStr"/>
+      <c r="CM118" t="n">
+        <v>219.38</v>
+      </c>
+      <c r="CN118" t="n">
+        <v>267.14</v>
+      </c>
+      <c r="CO118" t="n">
+        <v>196.39</v>
+      </c>
+      <c r="CP118" t="n">
+        <v>201.03</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
@@ -18535,9 +18589,15 @@
       </c>
       <c r="BB122" t="inlineStr"/>
       <c r="BC122" t="inlineStr"/>
-      <c r="BD122" t="inlineStr"/>
-      <c r="BE122" t="inlineStr"/>
-      <c r="BF122" t="inlineStr"/>
+      <c r="BD122" t="n">
+        <v>89.28</v>
+      </c>
+      <c r="BE122" t="n">
+        <v>95.84</v>
+      </c>
+      <c r="BF122" t="n">
+        <v>85.98</v>
+      </c>
       <c r="BG122" t="inlineStr"/>
       <c r="BH122" t="inlineStr"/>
       <c r="BI122" t="inlineStr"/>
@@ -18570,10 +18630,18 @@
       <c r="CJ122" t="inlineStr"/>
       <c r="CK122" t="inlineStr"/>
       <c r="CL122" t="inlineStr"/>
-      <c r="CM122" t="inlineStr"/>
-      <c r="CN122" t="inlineStr"/>
-      <c r="CO122" t="inlineStr"/>
-      <c r="CP122" t="inlineStr"/>
+      <c r="CM122" t="n">
+        <v>197.01</v>
+      </c>
+      <c r="CN122" t="n">
+        <v>205.89</v>
+      </c>
+      <c r="CO122" t="n">
+        <v>175.99</v>
+      </c>
+      <c r="CP122" t="n">
+        <v>190.2</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
@@ -19163,9 +19231,15 @@
       <c r="BK126" t="inlineStr"/>
       <c r="BL126" t="inlineStr"/>
       <c r="BM126" t="inlineStr"/>
-      <c r="BN126" t="inlineStr"/>
-      <c r="BO126" t="inlineStr"/>
-      <c r="BP126" t="inlineStr"/>
+      <c r="BN126" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO126" t="n">
+        <v>264.81</v>
+      </c>
+      <c r="BP126" t="n">
+        <v>916409.73</v>
+      </c>
       <c r="BQ126" t="inlineStr"/>
       <c r="BR126" t="inlineStr"/>
       <c r="BS126" t="inlineStr"/>
@@ -19188,10 +19262,18 @@
       <c r="CJ126" t="inlineStr"/>
       <c r="CK126" t="inlineStr"/>
       <c r="CL126" t="inlineStr"/>
-      <c r="CM126" t="inlineStr"/>
-      <c r="CN126" t="inlineStr"/>
-      <c r="CO126" t="inlineStr"/>
-      <c r="CP126" t="inlineStr"/>
+      <c r="CM126" t="n">
+        <v>162045.59</v>
+      </c>
+      <c r="CN126" t="n">
+        <v>40.04</v>
+      </c>
+      <c r="CO126" t="n">
+        <v>63.64</v>
+      </c>
+      <c r="CP126" t="n">
+        <v>9301.01</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
@@ -19321,9 +19403,15 @@
       <c r="BI127" t="inlineStr"/>
       <c r="BJ127" t="inlineStr"/>
       <c r="BK127" t="inlineStr"/>
-      <c r="BL127" t="inlineStr"/>
-      <c r="BM127" t="inlineStr"/>
-      <c r="BN127" t="inlineStr"/>
+      <c r="BL127" t="n">
+        <v>136.25</v>
+      </c>
+      <c r="BM127" t="n">
+        <v>131.73</v>
+      </c>
+      <c r="BN127" t="n">
+        <v>128.16</v>
+      </c>
       <c r="BO127" t="inlineStr"/>
       <c r="BP127" t="inlineStr"/>
       <c r="BQ127" t="inlineStr"/>
@@ -19348,10 +19436,18 @@
       <c r="CJ127" t="inlineStr"/>
       <c r="CK127" t="inlineStr"/>
       <c r="CL127" t="inlineStr"/>
-      <c r="CM127" t="inlineStr"/>
-      <c r="CN127" t="inlineStr"/>
-      <c r="CO127" t="inlineStr"/>
-      <c r="CP127" t="inlineStr"/>
+      <c r="CM127" t="n">
+        <v>153.64</v>
+      </c>
+      <c r="CN127" t="n">
+        <v>123.94</v>
+      </c>
+      <c r="CO127" t="n">
+        <v>86.31</v>
+      </c>
+      <c r="CP127" t="n">
+        <v>169.89</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
@@ -21559,10 +21655,18 @@
       <c r="BA142" t="n">
         <v>2004</v>
       </c>
-      <c r="BB142" t="inlineStr"/>
-      <c r="BC142" t="inlineStr"/>
-      <c r="BD142" t="inlineStr"/>
-      <c r="BE142" t="inlineStr"/>
+      <c r="BB142" t="n">
+        <v>2498.4</v>
+      </c>
+      <c r="BC142" t="n">
+        <v>2498.55</v>
+      </c>
+      <c r="BD142" t="n">
+        <v>2699.15</v>
+      </c>
+      <c r="BE142" t="n">
+        <v>2686.5</v>
+      </c>
       <c r="BF142" t="inlineStr"/>
       <c r="BG142" t="inlineStr"/>
       <c r="BH142" t="inlineStr"/>
@@ -21596,10 +21700,18 @@
       <c r="CJ142" t="inlineStr"/>
       <c r="CK142" t="inlineStr"/>
       <c r="CL142" t="inlineStr"/>
-      <c r="CM142" t="inlineStr"/>
-      <c r="CN142" t="inlineStr"/>
-      <c r="CO142" t="inlineStr"/>
-      <c r="CP142" t="inlineStr"/>
+      <c r="CM142" t="n">
+        <v>2685.72</v>
+      </c>
+      <c r="CN142" t="n">
+        <v>2685.01</v>
+      </c>
+      <c r="CO142" t="n">
+        <v>2646.44</v>
+      </c>
+      <c r="CP142" t="n">
+        <v>2645.41</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="n">
@@ -21701,10 +21813,18 @@
       <c r="BA143" t="n">
         <v>2004</v>
       </c>
-      <c r="BB143" t="inlineStr"/>
-      <c r="BC143" t="inlineStr"/>
-      <c r="BD143" t="inlineStr"/>
-      <c r="BE143" t="inlineStr"/>
+      <c r="BB143" t="n">
+        <v>14.32</v>
+      </c>
+      <c r="BC143" t="n">
+        <v>15.66</v>
+      </c>
+      <c r="BD143" t="n">
+        <v>42</v>
+      </c>
+      <c r="BE143" t="n">
+        <v>82.33</v>
+      </c>
       <c r="BF143" t="inlineStr"/>
       <c r="BG143" t="inlineStr"/>
       <c r="BH143" t="inlineStr"/>
@@ -21738,10 +21858,18 @@
       <c r="CJ143" t="inlineStr"/>
       <c r="CK143" t="inlineStr"/>
       <c r="CL143" t="inlineStr"/>
-      <c r="CM143" t="inlineStr"/>
-      <c r="CN143" t="inlineStr"/>
-      <c r="CO143" t="inlineStr"/>
-      <c r="CP143" t="inlineStr"/>
+      <c r="CM143" t="n">
+        <v>29.04</v>
+      </c>
+      <c r="CN143" t="n">
+        <v>22.62</v>
+      </c>
+      <c r="CO143" t="n">
+        <v>17.72</v>
+      </c>
+      <c r="CP143" t="n">
+        <v>15.28</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -21843,10 +21971,18 @@
       <c r="BA144" t="n">
         <v>2004</v>
       </c>
-      <c r="BB144" t="inlineStr"/>
-      <c r="BC144" t="inlineStr"/>
-      <c r="BD144" t="inlineStr"/>
-      <c r="BE144" t="inlineStr"/>
+      <c r="BB144" t="n">
+        <v>108.23</v>
+      </c>
+      <c r="BC144" t="n">
+        <v>118.76</v>
+      </c>
+      <c r="BD144" t="n">
+        <v>135.11</v>
+      </c>
+      <c r="BE144" t="n">
+        <v>96.3</v>
+      </c>
       <c r="BF144" t="inlineStr"/>
       <c r="BG144" t="inlineStr"/>
       <c r="BH144" t="inlineStr"/>
@@ -21880,10 +22016,18 @@
       <c r="CJ144" t="inlineStr"/>
       <c r="CK144" t="inlineStr"/>
       <c r="CL144" t="inlineStr"/>
-      <c r="CM144" t="inlineStr"/>
-      <c r="CN144" t="inlineStr"/>
-      <c r="CO144" t="inlineStr"/>
-      <c r="CP144" t="inlineStr"/>
+      <c r="CM144" t="n">
+        <v>100.18</v>
+      </c>
+      <c r="CN144" t="n">
+        <v>78.61</v>
+      </c>
+      <c r="CO144" t="n">
+        <v>90.25</v>
+      </c>
+      <c r="CP144" t="n">
+        <v>76.97</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -22275,10 +22419,18 @@
       <c r="BA147" t="n">
         <v>2003</v>
       </c>
-      <c r="BB147" t="inlineStr"/>
-      <c r="BC147" t="inlineStr"/>
-      <c r="BD147" t="inlineStr"/>
-      <c r="BE147" t="inlineStr"/>
+      <c r="BB147" t="n">
+        <v>211.04</v>
+      </c>
+      <c r="BC147" t="n">
+        <v>221.72</v>
+      </c>
+      <c r="BD147" t="n">
+        <v>348.95</v>
+      </c>
+      <c r="BE147" t="n">
+        <v>276.17</v>
+      </c>
       <c r="BF147" t="inlineStr"/>
       <c r="BG147" t="inlineStr"/>
       <c r="BH147" t="inlineStr"/>
@@ -22312,10 +22464,18 @@
       <c r="CJ147" t="inlineStr"/>
       <c r="CK147" t="inlineStr"/>
       <c r="CL147" t="inlineStr"/>
-      <c r="CM147" t="inlineStr"/>
-      <c r="CN147" t="inlineStr"/>
-      <c r="CO147" t="inlineStr"/>
-      <c r="CP147" t="inlineStr"/>
+      <c r="CM147" t="n">
+        <v>276.17</v>
+      </c>
+      <c r="CN147" t="n">
+        <v>336.54</v>
+      </c>
+      <c r="CO147" t="n">
+        <v>274.64</v>
+      </c>
+      <c r="CP147" t="n">
+        <v>169.06</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -22713,10 +22873,18 @@
       <c r="BA150" t="n">
         <v>2004</v>
       </c>
-      <c r="BB150" t="inlineStr"/>
-      <c r="BC150" t="inlineStr"/>
-      <c r="BD150" t="inlineStr"/>
-      <c r="BE150" t="inlineStr"/>
+      <c r="BB150" t="n">
+        <v>16.28</v>
+      </c>
+      <c r="BC150" t="n">
+        <v>8.050000000000001</v>
+      </c>
+      <c r="BD150" t="n">
+        <v>1.52</v>
+      </c>
+      <c r="BE150" t="n">
+        <v>2.17</v>
+      </c>
       <c r="BF150" t="inlineStr"/>
       <c r="BG150" t="inlineStr"/>
       <c r="BH150" t="inlineStr"/>
@@ -22750,10 +22918,18 @@
       <c r="CJ150" t="inlineStr"/>
       <c r="CK150" t="inlineStr"/>
       <c r="CL150" t="inlineStr"/>
-      <c r="CM150" t="inlineStr"/>
-      <c r="CN150" t="inlineStr"/>
-      <c r="CO150" t="inlineStr"/>
-      <c r="CP150" t="inlineStr"/>
+      <c r="CM150" t="n">
+        <v>2.17</v>
+      </c>
+      <c r="CN150" t="n">
+        <v>21.22</v>
+      </c>
+      <c r="CO150" t="n">
+        <v>11.93</v>
+      </c>
+      <c r="CP150" t="n">
+        <v>14.21</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="n">
@@ -24203,8 +24379,12 @@
       <c r="BE160" t="inlineStr"/>
       <c r="BF160" t="inlineStr"/>
       <c r="BG160" t="inlineStr"/>
-      <c r="BH160" t="inlineStr"/>
-      <c r="BI160" t="inlineStr"/>
+      <c r="BH160" t="n">
+        <v>48.8</v>
+      </c>
+      <c r="BI160" t="n">
+        <v>186.41</v>
+      </c>
       <c r="BJ160" t="inlineStr"/>
       <c r="BK160" t="inlineStr"/>
       <c r="BL160" t="inlineStr"/>
@@ -24234,10 +24414,18 @@
       <c r="CJ160" t="inlineStr"/>
       <c r="CK160" t="inlineStr"/>
       <c r="CL160" t="inlineStr"/>
-      <c r="CM160" t="inlineStr"/>
-      <c r="CN160" t="inlineStr"/>
-      <c r="CO160" t="inlineStr"/>
-      <c r="CP160" t="inlineStr"/>
+      <c r="CM160" t="n">
+        <v>196.13</v>
+      </c>
+      <c r="CN160" t="n">
+        <v>4.77</v>
+      </c>
+      <c r="CO160" t="n">
+        <v>3.52</v>
+      </c>
+      <c r="CP160" t="n">
+        <v>31.49</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="n">
@@ -25054,8 +25242,12 @@
       <c r="BB166" t="inlineStr"/>
       <c r="BC166" t="inlineStr"/>
       <c r="BD166" t="inlineStr"/>
-      <c r="BE166" t="inlineStr"/>
-      <c r="BF166" t="inlineStr"/>
+      <c r="BE166" t="n">
+        <v>2.77</v>
+      </c>
+      <c r="BF166" t="n">
+        <v>12.17</v>
+      </c>
       <c r="BG166" t="inlineStr"/>
       <c r="BH166" t="inlineStr"/>
       <c r="BI166" t="inlineStr"/>
@@ -25088,10 +25280,18 @@
       <c r="CJ166" t="inlineStr"/>
       <c r="CK166" t="inlineStr"/>
       <c r="CL166" t="inlineStr"/>
-      <c r="CM166" t="inlineStr"/>
-      <c r="CN166" t="inlineStr"/>
-      <c r="CO166" t="inlineStr"/>
-      <c r="CP166" t="inlineStr"/>
+      <c r="CM166" t="n">
+        <v>4.61</v>
+      </c>
+      <c r="CN166" t="n">
+        <v>2.08</v>
+      </c>
+      <c r="CO166" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="CP166" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="n">
@@ -25197,12 +25397,24 @@
       <c r="BA167" t="n">
         <v>2006</v>
       </c>
-      <c r="BB167" t="inlineStr"/>
-      <c r="BC167" t="inlineStr"/>
-      <c r="BD167" t="inlineStr"/>
-      <c r="BE167" t="inlineStr"/>
-      <c r="BF167" t="inlineStr"/>
-      <c r="BG167" t="inlineStr"/>
+      <c r="BB167" t="n">
+        <v>663.85</v>
+      </c>
+      <c r="BC167" t="n">
+        <v>341.79</v>
+      </c>
+      <c r="BD167" t="n">
+        <v>341.94</v>
+      </c>
+      <c r="BE167" t="n">
+        <v>342.01</v>
+      </c>
+      <c r="BF167" t="n">
+        <v>1056.26</v>
+      </c>
+      <c r="BG167" t="n">
+        <v>1056.47</v>
+      </c>
       <c r="BH167" t="inlineStr"/>
       <c r="BI167" t="inlineStr"/>
       <c r="BJ167" t="inlineStr"/>
@@ -25234,10 +25446,18 @@
       <c r="CJ167" t="inlineStr"/>
       <c r="CK167" t="inlineStr"/>
       <c r="CL167" t="inlineStr"/>
-      <c r="CM167" t="inlineStr"/>
-      <c r="CN167" t="inlineStr"/>
-      <c r="CO167" t="inlineStr"/>
-      <c r="CP167" t="inlineStr"/>
+      <c r="CM167" t="n">
+        <v>1251.03</v>
+      </c>
+      <c r="CN167" t="n">
+        <v>109.76</v>
+      </c>
+      <c r="CO167" t="n">
+        <v>1294.8</v>
+      </c>
+      <c r="CP167" t="n">
+        <v>124.96</v>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="n">
@@ -25349,12 +25569,24 @@
       </c>
       <c r="BB168" t="inlineStr"/>
       <c r="BC168" t="inlineStr"/>
-      <c r="BD168" t="inlineStr"/>
-      <c r="BE168" t="inlineStr"/>
-      <c r="BF168" t="inlineStr"/>
-      <c r="BG168" t="inlineStr"/>
-      <c r="BH168" t="inlineStr"/>
-      <c r="BI168" t="inlineStr"/>
+      <c r="BD168" t="n">
+        <v>111.88</v>
+      </c>
+      <c r="BE168" t="n">
+        <v>122.69</v>
+      </c>
+      <c r="BF168" t="n">
+        <v>131.08</v>
+      </c>
+      <c r="BG168" t="n">
+        <v>119.38</v>
+      </c>
+      <c r="BH168" t="n">
+        <v>73.20999999999999</v>
+      </c>
+      <c r="BI168" t="n">
+        <v>64.14</v>
+      </c>
       <c r="BJ168" t="inlineStr"/>
       <c r="BK168" t="inlineStr"/>
       <c r="BL168" t="inlineStr"/>
@@ -25384,10 +25616,18 @@
       <c r="CJ168" t="inlineStr"/>
       <c r="CK168" t="inlineStr"/>
       <c r="CL168" t="inlineStr"/>
-      <c r="CM168" t="inlineStr"/>
-      <c r="CN168" t="inlineStr"/>
-      <c r="CO168" t="inlineStr"/>
-      <c r="CP168" t="inlineStr"/>
+      <c r="CM168" t="n">
+        <v>220.76</v>
+      </c>
+      <c r="CN168" t="n">
+        <v>214.99</v>
+      </c>
+      <c r="CO168" t="n">
+        <v>194.93</v>
+      </c>
+      <c r="CP168" t="n">
+        <v>171.74</v>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="n">
@@ -26795,12 +27035,24 @@
       <c r="BK177" t="inlineStr"/>
       <c r="BL177" t="inlineStr"/>
       <c r="BM177" t="inlineStr"/>
-      <c r="BN177" t="inlineStr"/>
-      <c r="BO177" t="inlineStr"/>
-      <c r="BP177" t="inlineStr"/>
-      <c r="BQ177" t="inlineStr"/>
-      <c r="BR177" t="inlineStr"/>
-      <c r="BS177" t="inlineStr"/>
+      <c r="BN177" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO177" t="n">
+        <v>1139.91</v>
+      </c>
+      <c r="BP177" t="n">
+        <v>1181.23</v>
+      </c>
+      <c r="BQ177" t="n">
+        <v>1169.45</v>
+      </c>
+      <c r="BR177" t="n">
+        <v>122.18</v>
+      </c>
+      <c r="BS177" t="n">
+        <v>219</v>
+      </c>
       <c r="BT177" t="inlineStr"/>
       <c r="BU177" t="inlineStr"/>
       <c r="BV177" t="inlineStr"/>
@@ -26820,10 +27072,18 @@
       <c r="CJ177" t="inlineStr"/>
       <c r="CK177" t="inlineStr"/>
       <c r="CL177" t="inlineStr"/>
-      <c r="CM177" t="inlineStr"/>
-      <c r="CN177" t="inlineStr"/>
-      <c r="CO177" t="inlineStr"/>
-      <c r="CP177" t="inlineStr"/>
+      <c r="CM177" t="n">
+        <v>6568.45</v>
+      </c>
+      <c r="CN177" t="n">
+        <v>506.9</v>
+      </c>
+      <c r="CO177" t="n">
+        <v>464.68</v>
+      </c>
+      <c r="CP177" t="n">
+        <v>641</v>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="n">
@@ -29107,10 +29367,18 @@
       <c r="BA192" t="n">
         <v>2007</v>
       </c>
-      <c r="BB192" t="inlineStr"/>
-      <c r="BC192" t="inlineStr"/>
-      <c r="BD192" t="inlineStr"/>
-      <c r="BE192" t="inlineStr"/>
+      <c r="BB192" t="n">
+        <v>153.28</v>
+      </c>
+      <c r="BC192" t="n">
+        <v>156.48</v>
+      </c>
+      <c r="BD192" t="n">
+        <v>91.44</v>
+      </c>
+      <c r="BE192" t="n">
+        <v>95.17</v>
+      </c>
       <c r="BF192" t="inlineStr"/>
       <c r="BG192" t="inlineStr"/>
       <c r="BH192" t="inlineStr"/>
@@ -29144,10 +29412,18 @@
       <c r="CJ192" t="inlineStr"/>
       <c r="CK192" t="inlineStr"/>
       <c r="CL192" t="inlineStr"/>
-      <c r="CM192" t="inlineStr"/>
-      <c r="CN192" t="inlineStr"/>
-      <c r="CO192" t="inlineStr"/>
-      <c r="CP192" t="inlineStr"/>
+      <c r="CM192" t="n">
+        <v>95.17</v>
+      </c>
+      <c r="CN192" t="n">
+        <v>112.94</v>
+      </c>
+      <c r="CO192" t="n">
+        <v>123.52</v>
+      </c>
+      <c r="CP192" t="n">
+        <v>108.78</v>
+      </c>
     </row>
     <row r="193">
       <c r="A193" t="n">
@@ -29249,10 +29525,18 @@
       <c r="BA193" t="n">
         <v>2007</v>
       </c>
-      <c r="BB193" t="inlineStr"/>
-      <c r="BC193" t="inlineStr"/>
-      <c r="BD193" t="inlineStr"/>
-      <c r="BE193" t="inlineStr"/>
+      <c r="BB193" t="n">
+        <v>17.98</v>
+      </c>
+      <c r="BC193" t="n">
+        <v>17.98</v>
+      </c>
+      <c r="BD193" t="n">
+        <v>17.98</v>
+      </c>
+      <c r="BE193" t="n">
+        <v>17.98</v>
+      </c>
       <c r="BF193" t="inlineStr"/>
       <c r="BG193" t="inlineStr"/>
       <c r="BH193" t="inlineStr"/>
@@ -29286,10 +29570,18 @@
       <c r="CJ193" t="inlineStr"/>
       <c r="CK193" t="inlineStr"/>
       <c r="CL193" t="inlineStr"/>
-      <c r="CM193" t="inlineStr"/>
-      <c r="CN193" t="inlineStr"/>
-      <c r="CO193" t="inlineStr"/>
-      <c r="CP193" t="inlineStr"/>
+      <c r="CM193" t="n">
+        <v>17.98</v>
+      </c>
+      <c r="CN193" t="n">
+        <v>9248.67</v>
+      </c>
+      <c r="CO193" t="n">
+        <v>9267.91</v>
+      </c>
+      <c r="CP193" t="n">
+        <v>9267.91</v>
+      </c>
     </row>
     <row r="194">
       <c r="A194" t="n">
@@ -29997,10 +30289,18 @@
       <c r="BC198" t="inlineStr"/>
       <c r="BD198" t="inlineStr"/>
       <c r="BE198" t="inlineStr"/>
-      <c r="BF198" t="inlineStr"/>
-      <c r="BG198" t="inlineStr"/>
-      <c r="BH198" t="inlineStr"/>
-      <c r="BI198" t="inlineStr"/>
+      <c r="BF198" t="n">
+        <v>62.53</v>
+      </c>
+      <c r="BG198" t="n">
+        <v>57.25</v>
+      </c>
+      <c r="BH198" t="n">
+        <v>126.46</v>
+      </c>
+      <c r="BI198" t="n">
+        <v>280.45</v>
+      </c>
       <c r="BJ198" t="inlineStr"/>
       <c r="BK198" t="inlineStr"/>
       <c r="BL198" t="inlineStr"/>
@@ -30030,10 +30330,18 @@
       <c r="CJ198" t="inlineStr"/>
       <c r="CK198" t="inlineStr"/>
       <c r="CL198" t="inlineStr"/>
-      <c r="CM198" t="inlineStr"/>
-      <c r="CN198" t="inlineStr"/>
-      <c r="CO198" t="inlineStr"/>
-      <c r="CP198" t="inlineStr"/>
+      <c r="CM198" t="n">
+        <v>165.24</v>
+      </c>
+      <c r="CN198" t="n">
+        <v>150.74</v>
+      </c>
+      <c r="CO198" t="n">
+        <v>162.87</v>
+      </c>
+      <c r="CP198" t="n">
+        <v>152.63</v>
+      </c>
     </row>
     <row r="199">
       <c r="A199" t="n">
@@ -30156,10 +30464,18 @@
       <c r="BF199" t="inlineStr"/>
       <c r="BG199" t="inlineStr"/>
       <c r="BH199" t="inlineStr"/>
-      <c r="BI199" t="inlineStr"/>
-      <c r="BJ199" t="inlineStr"/>
-      <c r="BK199" t="inlineStr"/>
-      <c r="BL199" t="inlineStr"/>
+      <c r="BI199" t="n">
+        <v>663.85</v>
+      </c>
+      <c r="BJ199" t="n">
+        <v>341.79</v>
+      </c>
+      <c r="BK199" t="n">
+        <v>341.94</v>
+      </c>
+      <c r="BL199" t="n">
+        <v>342.01</v>
+      </c>
       <c r="BM199" t="inlineStr"/>
       <c r="BN199" t="inlineStr"/>
       <c r="BO199" t="inlineStr"/>
@@ -30186,10 +30502,18 @@
       <c r="CJ199" t="inlineStr"/>
       <c r="CK199" t="inlineStr"/>
       <c r="CL199" t="inlineStr"/>
-      <c r="CM199" t="inlineStr"/>
-      <c r="CN199" t="inlineStr"/>
-      <c r="CO199" t="inlineStr"/>
-      <c r="CP199" t="inlineStr"/>
+      <c r="CM199" t="n">
+        <v>1056.26</v>
+      </c>
+      <c r="CN199" t="n">
+        <v>1056.47</v>
+      </c>
+      <c r="CO199" t="n">
+        <v>1251.03</v>
+      </c>
+      <c r="CP199" t="n">
+        <v>109.76</v>
+      </c>
     </row>
     <row r="200">
       <c r="A200" t="n">
@@ -30581,10 +30905,18 @@
       <c r="BA202" t="n">
         <v>2005</v>
       </c>
-      <c r="BB202" t="inlineStr"/>
-      <c r="BC202" t="inlineStr"/>
-      <c r="BD202" t="inlineStr"/>
-      <c r="BE202" t="inlineStr"/>
+      <c r="BB202" t="n">
+        <v>183.44</v>
+      </c>
+      <c r="BC202" t="n">
+        <v>173.5</v>
+      </c>
+      <c r="BD202" t="n">
+        <v>185.62</v>
+      </c>
+      <c r="BE202" t="n">
+        <v>177.9</v>
+      </c>
       <c r="BF202" t="inlineStr"/>
       <c r="BG202" t="inlineStr"/>
       <c r="BH202" t="inlineStr"/>
@@ -30618,10 +30950,18 @@
       <c r="CJ202" t="inlineStr"/>
       <c r="CK202" t="inlineStr"/>
       <c r="CL202" t="inlineStr"/>
-      <c r="CM202" t="inlineStr"/>
-      <c r="CN202" t="inlineStr"/>
-      <c r="CO202" t="inlineStr"/>
-      <c r="CP202" t="inlineStr"/>
+      <c r="CM202" t="n">
+        <v>145.53</v>
+      </c>
+      <c r="CN202" t="n">
+        <v>99.56999999999999</v>
+      </c>
+      <c r="CO202" t="n">
+        <v>92.84</v>
+      </c>
+      <c r="CP202" t="n">
+        <v>219.63</v>
+      </c>
     </row>
     <row r="203">
       <c r="A203" t="n">
@@ -31016,8 +31356,12 @@
       <c r="BB205" t="inlineStr"/>
       <c r="BC205" t="inlineStr"/>
       <c r="BD205" t="inlineStr"/>
-      <c r="BE205" t="inlineStr"/>
-      <c r="BF205" t="inlineStr"/>
+      <c r="BE205" t="n">
+        <v>320.45</v>
+      </c>
+      <c r="BF205" t="n">
+        <v>285.8</v>
+      </c>
       <c r="BG205" t="inlineStr"/>
       <c r="BH205" t="inlineStr"/>
       <c r="BI205" t="inlineStr"/>
@@ -31050,10 +31394,18 @@
       <c r="CJ205" t="inlineStr"/>
       <c r="CK205" t="inlineStr"/>
       <c r="CL205" t="inlineStr"/>
-      <c r="CM205" t="inlineStr"/>
-      <c r="CN205" t="inlineStr"/>
-      <c r="CO205" t="inlineStr"/>
-      <c r="CP205" t="inlineStr"/>
+      <c r="CM205" t="n">
+        <v>114.08</v>
+      </c>
+      <c r="CN205" t="n">
+        <v>163.49</v>
+      </c>
+      <c r="CO205" t="n">
+        <v>143.32</v>
+      </c>
+      <c r="CP205" t="n">
+        <v>2216.12</v>
+      </c>
     </row>
     <row r="206">
       <c r="A206" t="n">
@@ -31631,12 +31983,24 @@
       <c r="BA209" t="n">
         <v>2006</v>
       </c>
-      <c r="BB209" t="inlineStr"/>
-      <c r="BC209" t="inlineStr"/>
-      <c r="BD209" t="inlineStr"/>
-      <c r="BE209" t="inlineStr"/>
-      <c r="BF209" t="inlineStr"/>
-      <c r="BG209" t="inlineStr"/>
+      <c r="BB209" t="n">
+        <v>28.41</v>
+      </c>
+      <c r="BC209" t="n">
+        <v>32.59</v>
+      </c>
+      <c r="BD209" t="n">
+        <v>46.65</v>
+      </c>
+      <c r="BE209" t="n">
+        <v>46.57</v>
+      </c>
+      <c r="BF209" t="n">
+        <v>42.63</v>
+      </c>
+      <c r="BG209" t="n">
+        <v>43.38</v>
+      </c>
       <c r="BH209" t="inlineStr"/>
       <c r="BI209" t="inlineStr"/>
       <c r="BJ209" t="inlineStr"/>
@@ -31668,10 +32032,18 @@
       <c r="CJ209" t="inlineStr"/>
       <c r="CK209" t="inlineStr"/>
       <c r="CL209" t="inlineStr"/>
-      <c r="CM209" t="inlineStr"/>
-      <c r="CN209" t="inlineStr"/>
-      <c r="CO209" t="inlineStr"/>
-      <c r="CP209" t="inlineStr"/>
+      <c r="CM209" t="n">
+        <v>48.17</v>
+      </c>
+      <c r="CN209" t="n">
+        <v>50.56</v>
+      </c>
+      <c r="CO209" t="n">
+        <v>48.31</v>
+      </c>
+      <c r="CP209" t="n">
+        <v>48.87</v>
+      </c>
     </row>
     <row r="210">
       <c r="A210" t="n">
@@ -31785,13 +32157,27 @@
       </c>
       <c r="BB210" t="inlineStr"/>
       <c r="BC210" t="inlineStr"/>
-      <c r="BD210" t="inlineStr"/>
-      <c r="BE210" t="inlineStr"/>
-      <c r="BF210" t="inlineStr"/>
-      <c r="BG210" t="inlineStr"/>
-      <c r="BH210" t="inlineStr"/>
-      <c r="BI210" t="inlineStr"/>
-      <c r="BJ210" t="inlineStr"/>
+      <c r="BD210" t="n">
+        <v>663.85</v>
+      </c>
+      <c r="BE210" t="n">
+        <v>341.79</v>
+      </c>
+      <c r="BF210" t="n">
+        <v>341.94</v>
+      </c>
+      <c r="BG210" t="n">
+        <v>342.01</v>
+      </c>
+      <c r="BH210" t="n">
+        <v>1056.26</v>
+      </c>
+      <c r="BI210" t="n">
+        <v>1056.47</v>
+      </c>
+      <c r="BJ210" t="n">
+        <v>1251.03</v>
+      </c>
       <c r="BK210" t="inlineStr"/>
       <c r="BL210" t="inlineStr"/>
       <c r="BM210" t="inlineStr"/>
@@ -31820,10 +32206,18 @@
       <c r="CJ210" t="inlineStr"/>
       <c r="CK210" t="inlineStr"/>
       <c r="CL210" t="inlineStr"/>
-      <c r="CM210" t="inlineStr"/>
-      <c r="CN210" t="inlineStr"/>
-      <c r="CO210" t="inlineStr"/>
-      <c r="CP210" t="inlineStr"/>
+      <c r="CM210" t="n">
+        <v>109.76</v>
+      </c>
+      <c r="CN210" t="n">
+        <v>1294.8</v>
+      </c>
+      <c r="CO210" t="n">
+        <v>124.96</v>
+      </c>
+      <c r="CP210" t="n">
+        <v>950.66</v>
+      </c>
     </row>
     <row r="211">
       <c r="A211" t="n">
@@ -32262,13 +32656,27 @@
       <c r="BF213" t="inlineStr"/>
       <c r="BG213" t="inlineStr"/>
       <c r="BH213" t="inlineStr"/>
-      <c r="BI213" t="inlineStr"/>
-      <c r="BJ213" t="inlineStr"/>
-      <c r="BK213" t="inlineStr"/>
-      <c r="BL213" t="inlineStr"/>
-      <c r="BM213" t="inlineStr"/>
-      <c r="BN213" t="inlineStr"/>
-      <c r="BO213" t="inlineStr"/>
+      <c r="BI213" t="n">
+        <v>444.25</v>
+      </c>
+      <c r="BJ213" t="n">
+        <v>459.86</v>
+      </c>
+      <c r="BK213" t="n">
+        <v>41.13</v>
+      </c>
+      <c r="BL213" t="n">
+        <v>33.33</v>
+      </c>
+      <c r="BM213" t="n">
+        <v>29.01</v>
+      </c>
+      <c r="BN213" t="n">
+        <v>126.98</v>
+      </c>
+      <c r="BO213" t="n">
+        <v>44.95</v>
+      </c>
       <c r="BP213" t="inlineStr"/>
       <c r="BQ213" t="inlineStr"/>
       <c r="BR213" t="inlineStr"/>
@@ -32292,10 +32700,18 @@
       <c r="CJ213" t="inlineStr"/>
       <c r="CK213" t="inlineStr"/>
       <c r="CL213" t="inlineStr"/>
-      <c r="CM213" t="inlineStr"/>
-      <c r="CN213" t="inlineStr"/>
-      <c r="CO213" t="inlineStr"/>
-      <c r="CP213" t="inlineStr"/>
+      <c r="CM213" t="n">
+        <v>54.16</v>
+      </c>
+      <c r="CN213" t="n">
+        <v>61.72</v>
+      </c>
+      <c r="CO213" t="n">
+        <v>22.18</v>
+      </c>
+      <c r="CP213" t="n">
+        <v>51.43</v>
+      </c>
     </row>
     <row r="214">
       <c r="A214" t="n">
@@ -32399,11 +32815,21 @@
       <c r="BA214" t="n">
         <v>2005</v>
       </c>
-      <c r="BB214" t="inlineStr"/>
-      <c r="BC214" t="inlineStr"/>
-      <c r="BD214" t="inlineStr"/>
-      <c r="BE214" t="inlineStr"/>
-      <c r="BF214" t="inlineStr"/>
+      <c r="BB214" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC214" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD214" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE214" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF214" t="n">
+        <v>0</v>
+      </c>
       <c r="BG214" t="inlineStr"/>
       <c r="BH214" t="inlineStr"/>
       <c r="BI214" t="inlineStr"/>
@@ -32436,10 +32862,18 @@
       <c r="CJ214" t="inlineStr"/>
       <c r="CK214" t="inlineStr"/>
       <c r="CL214" t="inlineStr"/>
-      <c r="CM214" t="inlineStr"/>
-      <c r="CN214" t="inlineStr"/>
-      <c r="CO214" t="inlineStr"/>
-      <c r="CP214" t="inlineStr"/>
+      <c r="CM214" t="n">
+        <v>224.46</v>
+      </c>
+      <c r="CN214" t="n">
+        <v>360.32</v>
+      </c>
+      <c r="CO214" t="n">
+        <v>340.1</v>
+      </c>
+      <c r="CP214" t="n">
+        <v>437.09</v>
+      </c>
     </row>
     <row r="215">
       <c r="A215" t="n">
@@ -32683,11 +33117,21 @@
       <c r="BA216" t="n">
         <v>2005</v>
       </c>
-      <c r="BB216" t="inlineStr"/>
-      <c r="BC216" t="inlineStr"/>
-      <c r="BD216" t="inlineStr"/>
-      <c r="BE216" t="inlineStr"/>
-      <c r="BF216" t="inlineStr"/>
+      <c r="BB216" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC216" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD216" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="BE216" t="n">
+        <v>1449.03</v>
+      </c>
+      <c r="BF216" t="n">
+        <v>1645.82</v>
+      </c>
       <c r="BG216" t="inlineStr"/>
       <c r="BH216" t="inlineStr"/>
       <c r="BI216" t="inlineStr"/>
@@ -32720,10 +33164,18 @@
       <c r="CJ216" t="inlineStr"/>
       <c r="CK216" t="inlineStr"/>
       <c r="CL216" t="inlineStr"/>
-      <c r="CM216" t="inlineStr"/>
-      <c r="CN216" t="inlineStr"/>
-      <c r="CO216" t="inlineStr"/>
-      <c r="CP216" t="inlineStr"/>
+      <c r="CM216" t="n">
+        <v>1657.11</v>
+      </c>
+      <c r="CN216" t="n">
+        <v>2112.05</v>
+      </c>
+      <c r="CO216" t="n">
+        <v>2114.11</v>
+      </c>
+      <c r="CP216" t="n">
+        <v>2803.51</v>
+      </c>
     </row>
     <row r="217">
       <c r="A217" t="n">
@@ -32977,11 +33429,21 @@
       </c>
       <c r="BB218" t="inlineStr"/>
       <c r="BC218" t="inlineStr"/>
-      <c r="BD218" t="inlineStr"/>
-      <c r="BE218" t="inlineStr"/>
-      <c r="BF218" t="inlineStr"/>
-      <c r="BG218" t="inlineStr"/>
-      <c r="BH218" t="inlineStr"/>
+      <c r="BD218" t="n">
+        <v>198.69</v>
+      </c>
+      <c r="BE218" t="n">
+        <v>192.92</v>
+      </c>
+      <c r="BF218" t="n">
+        <v>162.45</v>
+      </c>
+      <c r="BG218" t="n">
+        <v>156.54</v>
+      </c>
+      <c r="BH218" t="n">
+        <v>153.28</v>
+      </c>
       <c r="BI218" t="inlineStr"/>
       <c r="BJ218" t="inlineStr"/>
       <c r="BK218" t="inlineStr"/>
@@ -33012,10 +33474,18 @@
       <c r="CJ218" t="inlineStr"/>
       <c r="CK218" t="inlineStr"/>
       <c r="CL218" t="inlineStr"/>
-      <c r="CM218" t="inlineStr"/>
-      <c r="CN218" t="inlineStr"/>
-      <c r="CO218" t="inlineStr"/>
-      <c r="CP218" t="inlineStr"/>
+      <c r="CM218" t="n">
+        <v>156.48</v>
+      </c>
+      <c r="CN218" t="n">
+        <v>91.44</v>
+      </c>
+      <c r="CO218" t="n">
+        <v>95.17</v>
+      </c>
+      <c r="CP218" t="n">
+        <v>112.94</v>
+      </c>
     </row>
     <row r="219">
       <c r="A219" t="n">
@@ -33125,11 +33595,21 @@
       </c>
       <c r="BB219" t="inlineStr"/>
       <c r="BC219" t="inlineStr"/>
-      <c r="BD219" t="inlineStr"/>
-      <c r="BE219" t="inlineStr"/>
-      <c r="BF219" t="inlineStr"/>
-      <c r="BG219" t="inlineStr"/>
-      <c r="BH219" t="inlineStr"/>
+      <c r="BD219" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE219" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF219" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG219" t="n">
+        <v>18.4</v>
+      </c>
+      <c r="BH219" t="n">
+        <v>17.98</v>
+      </c>
       <c r="BI219" t="inlineStr"/>
       <c r="BJ219" t="inlineStr"/>
       <c r="BK219" t="inlineStr"/>
@@ -33160,10 +33640,18 @@
       <c r="CJ219" t="inlineStr"/>
       <c r="CK219" t="inlineStr"/>
       <c r="CL219" t="inlineStr"/>
-      <c r="CM219" t="inlineStr"/>
-      <c r="CN219" t="inlineStr"/>
-      <c r="CO219" t="inlineStr"/>
-      <c r="CP219" t="inlineStr"/>
+      <c r="CM219" t="n">
+        <v>17.98</v>
+      </c>
+      <c r="CN219" t="n">
+        <v>17.98</v>
+      </c>
+      <c r="CO219" t="n">
+        <v>17.98</v>
+      </c>
+      <c r="CP219" t="n">
+        <v>9248.67</v>
+      </c>
     </row>
     <row r="220">
       <c r="A220" t="n">
@@ -33405,11 +33893,21 @@
       <c r="BA221" t="n">
         <v>2009</v>
       </c>
-      <c r="BB221" t="inlineStr"/>
-      <c r="BC221" t="inlineStr"/>
-      <c r="BD221" t="inlineStr"/>
-      <c r="BE221" t="inlineStr"/>
-      <c r="BF221" t="inlineStr"/>
+      <c r="BB221" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC221" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD221" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE221" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF221" t="n">
+        <v>0</v>
+      </c>
       <c r="BG221" t="inlineStr"/>
       <c r="BH221" t="inlineStr"/>
       <c r="BI221" t="inlineStr"/>
@@ -33442,10 +33940,18 @@
       <c r="CJ221" t="inlineStr"/>
       <c r="CK221" t="inlineStr"/>
       <c r="CL221" t="inlineStr"/>
-      <c r="CM221" t="inlineStr"/>
-      <c r="CN221" t="inlineStr"/>
-      <c r="CO221" t="inlineStr"/>
-      <c r="CP221" t="inlineStr"/>
+      <c r="CM221" t="n">
+        <v>3800.33</v>
+      </c>
+      <c r="CN221" t="n">
+        <v>155.62</v>
+      </c>
+      <c r="CO221" t="n">
+        <v>138.06</v>
+      </c>
+      <c r="CP221" t="n">
+        <v>149.69</v>
+      </c>
     </row>
     <row r="222">
       <c r="A222" t="n">
@@ -33552,11 +34058,21 @@
         <v>2005</v>
       </c>
       <c r="BB222" t="inlineStr"/>
-      <c r="BC222" t="inlineStr"/>
-      <c r="BD222" t="inlineStr"/>
-      <c r="BE222" t="inlineStr"/>
-      <c r="BF222" t="inlineStr"/>
-      <c r="BG222" t="inlineStr"/>
+      <c r="BC222" t="n">
+        <v>11.81</v>
+      </c>
+      <c r="BD222" t="n">
+        <v>12.51</v>
+      </c>
+      <c r="BE222" t="n">
+        <v>16.73</v>
+      </c>
+      <c r="BF222" t="n">
+        <v>57.95</v>
+      </c>
+      <c r="BG222" t="n">
+        <v>59.06</v>
+      </c>
       <c r="BH222" t="inlineStr"/>
       <c r="BI222" t="inlineStr"/>
       <c r="BJ222" t="inlineStr"/>
@@ -33588,10 +34104,18 @@
       <c r="CJ222" t="inlineStr"/>
       <c r="CK222" t="inlineStr"/>
       <c r="CL222" t="inlineStr"/>
-      <c r="CM222" t="inlineStr"/>
-      <c r="CN222" t="inlineStr"/>
-      <c r="CO222" t="inlineStr"/>
-      <c r="CP222" t="inlineStr"/>
+      <c r="CM222" t="n">
+        <v>53.63</v>
+      </c>
+      <c r="CN222" t="n">
+        <v>52.33</v>
+      </c>
+      <c r="CO222" t="n">
+        <v>51.75</v>
+      </c>
+      <c r="CP222" t="n">
+        <v>55.37</v>
+      </c>
     </row>
     <row r="223">
       <c r="A223" t="n">
@@ -33698,11 +34222,21 @@
         <v>2005</v>
       </c>
       <c r="BB223" t="inlineStr"/>
-      <c r="BC223" t="inlineStr"/>
-      <c r="BD223" t="inlineStr"/>
-      <c r="BE223" t="inlineStr"/>
-      <c r="BF223" t="inlineStr"/>
-      <c r="BG223" t="inlineStr"/>
+      <c r="BC223" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD223" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE223" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF223" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="BG223" t="n">
+        <v>9.630000000000001</v>
+      </c>
       <c r="BH223" t="inlineStr"/>
       <c r="BI223" t="inlineStr"/>
       <c r="BJ223" t="inlineStr"/>
@@ -33734,10 +34268,18 @@
       <c r="CJ223" t="inlineStr"/>
       <c r="CK223" t="inlineStr"/>
       <c r="CL223" t="inlineStr"/>
-      <c r="CM223" t="inlineStr"/>
-      <c r="CN223" t="inlineStr"/>
-      <c r="CO223" t="inlineStr"/>
-      <c r="CP223" t="inlineStr"/>
+      <c r="CM223" t="n">
+        <v>29.48</v>
+      </c>
+      <c r="CN223" t="n">
+        <v>12.95</v>
+      </c>
+      <c r="CO223" t="n">
+        <v>10.82</v>
+      </c>
+      <c r="CP223" t="n">
+        <v>21.26</v>
+      </c>
     </row>
     <row r="224">
       <c r="A224" t="n">
@@ -33986,11 +34528,21 @@
         <v>2005</v>
       </c>
       <c r="BB225" t="inlineStr"/>
-      <c r="BC225" t="inlineStr"/>
-      <c r="BD225" t="inlineStr"/>
-      <c r="BE225" t="inlineStr"/>
-      <c r="BF225" t="inlineStr"/>
-      <c r="BG225" t="inlineStr"/>
+      <c r="BC225" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD225" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE225" t="n">
+        <v>4420.92</v>
+      </c>
+      <c r="BF225" t="n">
+        <v>4420.92</v>
+      </c>
+      <c r="BG225" t="n">
+        <v>0</v>
+      </c>
       <c r="BH225" t="inlineStr"/>
       <c r="BI225" t="inlineStr"/>
       <c r="BJ225" t="inlineStr"/>
@@ -34022,10 +34574,18 @@
       <c r="CJ225" t="inlineStr"/>
       <c r="CK225" t="inlineStr"/>
       <c r="CL225" t="inlineStr"/>
-      <c r="CM225" t="inlineStr"/>
-      <c r="CN225" t="inlineStr"/>
-      <c r="CO225" t="inlineStr"/>
-      <c r="CP225" t="inlineStr"/>
+      <c r="CM225" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN225" t="n">
+        <v>0</v>
+      </c>
+      <c r="CO225" t="n">
+        <v>0</v>
+      </c>
+      <c r="CP225" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="226">
       <c r="A226" t="n">
@@ -34132,11 +34692,21 @@
         <v>2005</v>
       </c>
       <c r="BB226" t="inlineStr"/>
-      <c r="BC226" t="inlineStr"/>
-      <c r="BD226" t="inlineStr"/>
-      <c r="BE226" t="inlineStr"/>
-      <c r="BF226" t="inlineStr"/>
-      <c r="BG226" t="inlineStr"/>
+      <c r="BC226" t="n">
+        <v>199.39</v>
+      </c>
+      <c r="BD226" t="n">
+        <v>208.36</v>
+      </c>
+      <c r="BE226" t="n">
+        <v>214.86</v>
+      </c>
+      <c r="BF226" t="n">
+        <v>223.98</v>
+      </c>
+      <c r="BG226" t="n">
+        <v>221.12</v>
+      </c>
       <c r="BH226" t="inlineStr"/>
       <c r="BI226" t="inlineStr"/>
       <c r="BJ226" t="inlineStr"/>
@@ -34168,10 +34738,18 @@
       <c r="CJ226" t="inlineStr"/>
       <c r="CK226" t="inlineStr"/>
       <c r="CL226" t="inlineStr"/>
-      <c r="CM226" t="inlineStr"/>
-      <c r="CN226" t="inlineStr"/>
-      <c r="CO226" t="inlineStr"/>
-      <c r="CP226" t="inlineStr"/>
+      <c r="CM226" t="n">
+        <v>187.21</v>
+      </c>
+      <c r="CN226" t="n">
+        <v>140.06</v>
+      </c>
+      <c r="CO226" t="n">
+        <v>130.46</v>
+      </c>
+      <c r="CP226" t="n">
+        <v>169.96</v>
+      </c>
     </row>
     <row r="227">
       <c r="A227" t="n">
@@ -34420,11 +34998,21 @@
         <v>2005</v>
       </c>
       <c r="BB228" t="inlineStr"/>
-      <c r="BC228" t="inlineStr"/>
-      <c r="BD228" t="inlineStr"/>
-      <c r="BE228" t="inlineStr"/>
-      <c r="BF228" t="inlineStr"/>
-      <c r="BG228" t="inlineStr"/>
+      <c r="BC228" t="n">
+        <v>70.97</v>
+      </c>
+      <c r="BD228" t="n">
+        <v>67.62</v>
+      </c>
+      <c r="BE228" t="n">
+        <v>63.14</v>
+      </c>
+      <c r="BF228" t="n">
+        <v>61.27</v>
+      </c>
+      <c r="BG228" t="n">
+        <v>36.2</v>
+      </c>
       <c r="BH228" t="inlineStr"/>
       <c r="BI228" t="inlineStr"/>
       <c r="BJ228" t="inlineStr"/>
@@ -34456,10 +35044,18 @@
       <c r="CJ228" t="inlineStr"/>
       <c r="CK228" t="inlineStr"/>
       <c r="CL228" t="inlineStr"/>
-      <c r="CM228" t="inlineStr"/>
-      <c r="CN228" t="inlineStr"/>
-      <c r="CO228" t="inlineStr"/>
-      <c r="CP228" t="inlineStr"/>
+      <c r="CM228" t="n">
+        <v>51.56</v>
+      </c>
+      <c r="CN228" t="n">
+        <v>38.99</v>
+      </c>
+      <c r="CO228" t="n">
+        <v>36.92</v>
+      </c>
+      <c r="CP228" t="n">
+        <v>42.73</v>
+      </c>
     </row>
     <row r="229">
       <c r="A229" t="n">
@@ -35031,9 +35627,15 @@
       </c>
       <c r="BB232" t="inlineStr"/>
       <c r="BC232" t="inlineStr"/>
-      <c r="BD232" t="inlineStr"/>
-      <c r="BE232" t="inlineStr"/>
-      <c r="BF232" t="inlineStr"/>
+      <c r="BD232" t="n">
+        <v>297.04</v>
+      </c>
+      <c r="BE232" t="n">
+        <v>183.59</v>
+      </c>
+      <c r="BF232" t="n">
+        <v>263.55</v>
+      </c>
       <c r="BG232" t="inlineStr"/>
       <c r="BH232" t="inlineStr"/>
       <c r="BI232" t="inlineStr"/>
@@ -35066,10 +35668,18 @@
       <c r="CJ232" t="inlineStr"/>
       <c r="CK232" t="inlineStr"/>
       <c r="CL232" t="inlineStr"/>
-      <c r="CM232" t="inlineStr"/>
-      <c r="CN232" t="inlineStr"/>
-      <c r="CO232" t="inlineStr"/>
-      <c r="CP232" t="inlineStr"/>
+      <c r="CM232" t="n">
+        <v>324.2</v>
+      </c>
+      <c r="CN232" t="n">
+        <v>280.32</v>
+      </c>
+      <c r="CO232" t="n">
+        <v>327.77</v>
+      </c>
+      <c r="CP232" t="n">
+        <v>363.14</v>
+      </c>
     </row>
     <row r="233">
       <c r="A233" t="n">
@@ -35174,10 +35784,18 @@
         <v>2004</v>
       </c>
       <c r="BB233" t="inlineStr"/>
-      <c r="BC233" t="inlineStr"/>
-      <c r="BD233" t="inlineStr"/>
-      <c r="BE233" t="inlineStr"/>
-      <c r="BF233" t="inlineStr"/>
+      <c r="BC233" t="n">
+        <v>313.24</v>
+      </c>
+      <c r="BD233" t="n">
+        <v>283.67</v>
+      </c>
+      <c r="BE233" t="n">
+        <v>170.89</v>
+      </c>
+      <c r="BF233" t="n">
+        <v>276.8</v>
+      </c>
       <c r="BG233" t="inlineStr"/>
       <c r="BH233" t="inlineStr"/>
       <c r="BI233" t="inlineStr"/>
@@ -35210,10 +35828,18 @@
       <c r="CJ233" t="inlineStr"/>
       <c r="CK233" t="inlineStr"/>
       <c r="CL233" t="inlineStr"/>
-      <c r="CM233" t="inlineStr"/>
-      <c r="CN233" t="inlineStr"/>
-      <c r="CO233" t="inlineStr"/>
-      <c r="CP233" t="inlineStr"/>
+      <c r="CM233" t="n">
+        <v>410.98</v>
+      </c>
+      <c r="CN233" t="n">
+        <v>423.28</v>
+      </c>
+      <c r="CO233" t="n">
+        <v>461.5</v>
+      </c>
+      <c r="CP233" t="n">
+        <v>463.58</v>
+      </c>
     </row>
     <row r="234">
       <c r="A234" t="n">
@@ -35318,10 +35944,18 @@
         <v>2004</v>
       </c>
       <c r="BB234" t="inlineStr"/>
-      <c r="BC234" t="inlineStr"/>
-      <c r="BD234" t="inlineStr"/>
-      <c r="BE234" t="inlineStr"/>
-      <c r="BF234" t="inlineStr"/>
+      <c r="BC234" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD234" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE234" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF234" t="n">
+        <v>5061.24</v>
+      </c>
       <c r="BG234" t="inlineStr"/>
       <c r="BH234" t="inlineStr"/>
       <c r="BI234" t="inlineStr"/>
@@ -35354,10 +35988,18 @@
       <c r="CJ234" t="inlineStr"/>
       <c r="CK234" t="inlineStr"/>
       <c r="CL234" t="inlineStr"/>
-      <c r="CM234" t="inlineStr"/>
-      <c r="CN234" t="inlineStr"/>
-      <c r="CO234" t="inlineStr"/>
-      <c r="CP234" t="inlineStr"/>
+      <c r="CM234" t="n">
+        <v>4124.97</v>
+      </c>
+      <c r="CN234" t="n">
+        <v>1294.96</v>
+      </c>
+      <c r="CO234" t="n">
+        <v>1219.01</v>
+      </c>
+      <c r="CP234" t="n">
+        <v>427.24</v>
+      </c>
     </row>
     <row r="235">
       <c r="A235" t="n">
@@ -35462,10 +36104,18 @@
         <v>2004</v>
       </c>
       <c r="BB235" t="inlineStr"/>
-      <c r="BC235" t="inlineStr"/>
-      <c r="BD235" t="inlineStr"/>
-      <c r="BE235" t="inlineStr"/>
-      <c r="BF235" t="inlineStr"/>
+      <c r="BC235" t="n">
+        <v>214.06</v>
+      </c>
+      <c r="BD235" t="n">
+        <v>151.52</v>
+      </c>
+      <c r="BE235" t="n">
+        <v>5016.63</v>
+      </c>
+      <c r="BF235" t="n">
+        <v>108.53</v>
+      </c>
       <c r="BG235" t="inlineStr"/>
       <c r="BH235" t="inlineStr"/>
       <c r="BI235" t="inlineStr"/>
@@ -35498,10 +36148,18 @@
       <c r="CJ235" t="inlineStr"/>
       <c r="CK235" t="inlineStr"/>
       <c r="CL235" t="inlineStr"/>
-      <c r="CM235" t="inlineStr"/>
-      <c r="CN235" t="inlineStr"/>
-      <c r="CO235" t="inlineStr"/>
-      <c r="CP235" t="inlineStr"/>
+      <c r="CM235" t="n">
+        <v>148.96</v>
+      </c>
+      <c r="CN235" t="n">
+        <v>83.06</v>
+      </c>
+      <c r="CO235" t="n">
+        <v>81.22</v>
+      </c>
+      <c r="CP235" t="n">
+        <v>85.47</v>
+      </c>
     </row>
     <row r="236">
       <c r="A236" t="n">
@@ -35603,10 +36261,18 @@
       <c r="BA236" t="n">
         <v>2004</v>
       </c>
-      <c r="BB236" t="inlineStr"/>
-      <c r="BC236" t="inlineStr"/>
-      <c r="BD236" t="inlineStr"/>
-      <c r="BE236" t="inlineStr"/>
+      <c r="BB236" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC236" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD236" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE236" t="n">
+        <v>0</v>
+      </c>
       <c r="BF236" t="inlineStr"/>
       <c r="BG236" t="inlineStr"/>
       <c r="BH236" t="inlineStr"/>
@@ -35640,10 +36306,18 @@
       <c r="CJ236" t="inlineStr"/>
       <c r="CK236" t="inlineStr"/>
       <c r="CL236" t="inlineStr"/>
-      <c r="CM236" t="inlineStr"/>
-      <c r="CN236" t="inlineStr"/>
-      <c r="CO236" t="inlineStr"/>
-      <c r="CP236" t="inlineStr"/>
+      <c r="CM236" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN236" t="n">
+        <v>0</v>
+      </c>
+      <c r="CO236" t="n">
+        <v>0</v>
+      </c>
+      <c r="CP236" t="n">
+        <v>1252.4</v>
+      </c>
     </row>
     <row r="237">
       <c r="A237" t="n">
@@ -35748,10 +36422,18 @@
         <v>2004</v>
       </c>
       <c r="BB237" t="inlineStr"/>
-      <c r="BC237" t="inlineStr"/>
-      <c r="BD237" t="inlineStr"/>
-      <c r="BE237" t="inlineStr"/>
-      <c r="BF237" t="inlineStr"/>
+      <c r="BC237" t="n">
+        <v>97.33</v>
+      </c>
+      <c r="BD237" t="n">
+        <v>119.38</v>
+      </c>
+      <c r="BE237" t="n">
+        <v>58.05</v>
+      </c>
+      <c r="BF237" t="n">
+        <v>79.31</v>
+      </c>
       <c r="BG237" t="inlineStr"/>
       <c r="BH237" t="inlineStr"/>
       <c r="BI237" t="inlineStr"/>
@@ -35784,10 +36466,18 @@
       <c r="CJ237" t="inlineStr"/>
       <c r="CK237" t="inlineStr"/>
       <c r="CL237" t="inlineStr"/>
-      <c r="CM237" t="inlineStr"/>
-      <c r="CN237" t="inlineStr"/>
-      <c r="CO237" t="inlineStr"/>
-      <c r="CP237" t="inlineStr"/>
+      <c r="CM237" t="n">
+        <v>98.02</v>
+      </c>
+      <c r="CN237" t="n">
+        <v>87.29000000000001</v>
+      </c>
+      <c r="CO237" t="n">
+        <v>163.84</v>
+      </c>
+      <c r="CP237" t="n">
+        <v>134.22</v>
+      </c>
     </row>
     <row r="238">
       <c r="A238" t="n">
@@ -35892,10 +36582,18 @@
         <v>2004</v>
       </c>
       <c r="BB238" t="inlineStr"/>
-      <c r="BC238" t="inlineStr"/>
-      <c r="BD238" t="inlineStr"/>
-      <c r="BE238" t="inlineStr"/>
-      <c r="BF238" t="inlineStr"/>
+      <c r="BC238" t="n">
+        <v>38.08</v>
+      </c>
+      <c r="BD238" t="n">
+        <v>46.19</v>
+      </c>
+      <c r="BE238" t="n">
+        <v>66.56999999999999</v>
+      </c>
+      <c r="BF238" t="n">
+        <v>84.64</v>
+      </c>
       <c r="BG238" t="inlineStr"/>
       <c r="BH238" t="inlineStr"/>
       <c r="BI238" t="inlineStr"/>
@@ -35928,10 +36626,18 @@
       <c r="CJ238" t="inlineStr"/>
       <c r="CK238" t="inlineStr"/>
       <c r="CL238" t="inlineStr"/>
-      <c r="CM238" t="inlineStr"/>
-      <c r="CN238" t="inlineStr"/>
-      <c r="CO238" t="inlineStr"/>
-      <c r="CP238" t="inlineStr"/>
+      <c r="CM238" t="n">
+        <v>78.88</v>
+      </c>
+      <c r="CN238" t="n">
+        <v>83.89</v>
+      </c>
+      <c r="CO238" t="n">
+        <v>101.26</v>
+      </c>
+      <c r="CP238" t="n">
+        <v>108.05</v>
+      </c>
     </row>
     <row r="239">
       <c r="A239" t="n">
@@ -36036,10 +36742,18 @@
         <v>2004</v>
       </c>
       <c r="BB239" t="inlineStr"/>
-      <c r="BC239" t="inlineStr"/>
-      <c r="BD239" t="inlineStr"/>
-      <c r="BE239" t="inlineStr"/>
-      <c r="BF239" t="inlineStr"/>
+      <c r="BC239" t="n">
+        <v>70.97</v>
+      </c>
+      <c r="BD239" t="n">
+        <v>67.62</v>
+      </c>
+      <c r="BE239" t="n">
+        <v>63.14</v>
+      </c>
+      <c r="BF239" t="n">
+        <v>61.27</v>
+      </c>
       <c r="BG239" t="inlineStr"/>
       <c r="BH239" t="inlineStr"/>
       <c r="BI239" t="inlineStr"/>
@@ -36072,10 +36786,18 @@
       <c r="CJ239" t="inlineStr"/>
       <c r="CK239" t="inlineStr"/>
       <c r="CL239" t="inlineStr"/>
-      <c r="CM239" t="inlineStr"/>
-      <c r="CN239" t="inlineStr"/>
-      <c r="CO239" t="inlineStr"/>
-      <c r="CP239" t="inlineStr"/>
+      <c r="CM239" t="n">
+        <v>36.2</v>
+      </c>
+      <c r="CN239" t="n">
+        <v>51.56</v>
+      </c>
+      <c r="CO239" t="n">
+        <v>38.99</v>
+      </c>
+      <c r="CP239" t="n">
+        <v>36.92</v>
+      </c>
     </row>
     <row r="240">
       <c r="A240" t="n">
@@ -36180,10 +36902,18 @@
         <v>2004</v>
       </c>
       <c r="BB240" t="inlineStr"/>
-      <c r="BC240" t="inlineStr"/>
-      <c r="BD240" t="inlineStr"/>
-      <c r="BE240" t="inlineStr"/>
-      <c r="BF240" t="inlineStr"/>
+      <c r="BC240" t="n">
+        <v>88.03</v>
+      </c>
+      <c r="BD240" t="n">
+        <v>89.59999999999999</v>
+      </c>
+      <c r="BE240" t="n">
+        <v>67.45</v>
+      </c>
+      <c r="BF240" t="n">
+        <v>71.3</v>
+      </c>
       <c r="BG240" t="inlineStr"/>
       <c r="BH240" t="inlineStr"/>
       <c r="BI240" t="inlineStr"/>
@@ -36216,10 +36946,18 @@
       <c r="CJ240" t="inlineStr"/>
       <c r="CK240" t="inlineStr"/>
       <c r="CL240" t="inlineStr"/>
-      <c r="CM240" t="inlineStr"/>
-      <c r="CN240" t="inlineStr"/>
-      <c r="CO240" t="inlineStr"/>
-      <c r="CP240" t="inlineStr"/>
+      <c r="CM240" t="n">
+        <v>67.76000000000001</v>
+      </c>
+      <c r="CN240" t="n">
+        <v>71.62</v>
+      </c>
+      <c r="CO240" t="n">
+        <v>60.81</v>
+      </c>
+      <c r="CP240" t="n">
+        <v>60.99</v>
+      </c>
     </row>
     <row r="241">
       <c r="A241" t="n">
@@ -36321,10 +37059,18 @@
       <c r="BA241" t="n">
         <v>2004</v>
       </c>
-      <c r="BB241" t="inlineStr"/>
-      <c r="BC241" t="inlineStr"/>
-      <c r="BD241" t="inlineStr"/>
-      <c r="BE241" t="inlineStr"/>
+      <c r="BB241" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC241" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD241" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="BE241" t="n">
+        <v>2772.36</v>
+      </c>
       <c r="BF241" t="inlineStr"/>
       <c r="BG241" t="inlineStr"/>
       <c r="BH241" t="inlineStr"/>
@@ -36358,10 +37104,18 @@
       <c r="CJ241" t="inlineStr"/>
       <c r="CK241" t="inlineStr"/>
       <c r="CL241" t="inlineStr"/>
-      <c r="CM241" t="inlineStr"/>
-      <c r="CN241" t="inlineStr"/>
-      <c r="CO241" t="inlineStr"/>
-      <c r="CP241" t="inlineStr"/>
+      <c r="CM241" t="n">
+        <v>2772.36</v>
+      </c>
+      <c r="CN241" t="n">
+        <v>2300.21</v>
+      </c>
+      <c r="CO241" t="n">
+        <v>2093.87</v>
+      </c>
+      <c r="CP241" t="n">
+        <v>2047.32</v>
+      </c>
     </row>
     <row r="242">
       <c r="A242" t="n">
@@ -36801,10 +37555,18 @@
       </c>
       <c r="BB244" t="inlineStr"/>
       <c r="BC244" t="inlineStr"/>
-      <c r="BD244" t="inlineStr"/>
-      <c r="BE244" t="inlineStr"/>
-      <c r="BF244" t="inlineStr"/>
-      <c r="BG244" t="inlineStr"/>
+      <c r="BD244" t="n">
+        <v>2569.36</v>
+      </c>
+      <c r="BE244" t="n">
+        <v>2339.92</v>
+      </c>
+      <c r="BF244" t="n">
+        <v>1671.67</v>
+      </c>
+      <c r="BG244" t="n">
+        <v>1677.95</v>
+      </c>
       <c r="BH244" t="inlineStr"/>
       <c r="BI244" t="inlineStr"/>
       <c r="BJ244" t="inlineStr"/>
@@ -36836,10 +37598,18 @@
       <c r="CJ244" t="inlineStr"/>
       <c r="CK244" t="inlineStr"/>
       <c r="CL244" t="inlineStr"/>
-      <c r="CM244" t="inlineStr"/>
-      <c r="CN244" t="inlineStr"/>
-      <c r="CO244" t="inlineStr"/>
-      <c r="CP244" t="inlineStr"/>
+      <c r="CM244" t="n">
+        <v>1615.54</v>
+      </c>
+      <c r="CN244" t="n">
+        <v>1635.41</v>
+      </c>
+      <c r="CO244" t="n">
+        <v>1642.23</v>
+      </c>
+      <c r="CP244" t="n">
+        <v>1615.78</v>
+      </c>
     </row>
     <row r="245">
       <c r="A245" t="n">
@@ -37241,14 +38011,30 @@
       <c r="BA247" t="n">
         <v>2008</v>
       </c>
-      <c r="BB247" t="inlineStr"/>
-      <c r="BC247" t="inlineStr"/>
-      <c r="BD247" t="inlineStr"/>
-      <c r="BE247" t="inlineStr"/>
-      <c r="BF247" t="inlineStr"/>
-      <c r="BG247" t="inlineStr"/>
-      <c r="BH247" t="inlineStr"/>
-      <c r="BI247" t="inlineStr"/>
+      <c r="BB247" t="n">
+        <v>314.31</v>
+      </c>
+      <c r="BC247" t="n">
+        <v>78.77</v>
+      </c>
+      <c r="BD247" t="n">
+        <v>101.77</v>
+      </c>
+      <c r="BE247" t="n">
+        <v>115.74</v>
+      </c>
+      <c r="BF247" t="n">
+        <v>156.84</v>
+      </c>
+      <c r="BG247" t="n">
+        <v>261.15</v>
+      </c>
+      <c r="BH247" t="n">
+        <v>341.18</v>
+      </c>
+      <c r="BI247" t="n">
+        <v>184.29</v>
+      </c>
       <c r="BJ247" t="inlineStr"/>
       <c r="BK247" t="inlineStr"/>
       <c r="BL247" t="inlineStr"/>
@@ -37278,10 +38064,18 @@
       <c r="CJ247" t="inlineStr"/>
       <c r="CK247" t="inlineStr"/>
       <c r="CL247" t="inlineStr"/>
-      <c r="CM247" t="inlineStr"/>
-      <c r="CN247" t="inlineStr"/>
-      <c r="CO247" t="inlineStr"/>
-      <c r="CP247" t="inlineStr"/>
+      <c r="CM247" t="n">
+        <v>186.81</v>
+      </c>
+      <c r="CN247" t="n">
+        <v>218.11</v>
+      </c>
+      <c r="CO247" t="n">
+        <v>330.4</v>
+      </c>
+      <c r="CP247" t="n">
+        <v>324.82</v>
+      </c>
     </row>
     <row r="248">
       <c r="A248" t="n">
@@ -37391,14 +38185,30 @@
       <c r="BA248" t="n">
         <v>2008</v>
       </c>
-      <c r="BB248" t="inlineStr"/>
-      <c r="BC248" t="inlineStr"/>
-      <c r="BD248" t="inlineStr"/>
-      <c r="BE248" t="inlineStr"/>
-      <c r="BF248" t="inlineStr"/>
-      <c r="BG248" t="inlineStr"/>
-      <c r="BH248" t="inlineStr"/>
-      <c r="BI248" t="inlineStr"/>
+      <c r="BB248" t="n">
+        <v>611.62</v>
+      </c>
+      <c r="BC248" t="n">
+        <v>2669.68</v>
+      </c>
+      <c r="BD248" t="n">
+        <v>2675.88</v>
+      </c>
+      <c r="BE248" t="n">
+        <v>2753.2</v>
+      </c>
+      <c r="BF248" t="n">
+        <v>2771.46</v>
+      </c>
+      <c r="BG248" t="n">
+        <v>2758.94</v>
+      </c>
+      <c r="BH248" t="n">
+        <v>2784.32</v>
+      </c>
+      <c r="BI248" t="n">
+        <v>2741.65</v>
+      </c>
       <c r="BJ248" t="inlineStr"/>
       <c r="BK248" t="inlineStr"/>
       <c r="BL248" t="inlineStr"/>
@@ -37428,10 +38238,18 @@
       <c r="CJ248" t="inlineStr"/>
       <c r="CK248" t="inlineStr"/>
       <c r="CL248" t="inlineStr"/>
-      <c r="CM248" t="inlineStr"/>
-      <c r="CN248" t="inlineStr"/>
-      <c r="CO248" t="inlineStr"/>
-      <c r="CP248" t="inlineStr"/>
+      <c r="CM248" t="n">
+        <v>2796</v>
+      </c>
+      <c r="CN248" t="n">
+        <v>2060.65</v>
+      </c>
+      <c r="CO248" t="n">
+        <v>2066.15</v>
+      </c>
+      <c r="CP248" t="n">
+        <v>2088.03</v>
+      </c>
     </row>
     <row r="249">
       <c r="A249" t="n">
@@ -37541,14 +38359,30 @@
       <c r="BA249" t="n">
         <v>2008</v>
       </c>
-      <c r="BB249" t="inlineStr"/>
-      <c r="BC249" t="inlineStr"/>
-      <c r="BD249" t="inlineStr"/>
-      <c r="BE249" t="inlineStr"/>
-      <c r="BF249" t="inlineStr"/>
-      <c r="BG249" t="inlineStr"/>
-      <c r="BH249" t="inlineStr"/>
-      <c r="BI249" t="inlineStr"/>
+      <c r="BB249" t="n">
+        <v>816.38</v>
+      </c>
+      <c r="BC249" t="n">
+        <v>891.54</v>
+      </c>
+      <c r="BD249" t="n">
+        <v>854.04</v>
+      </c>
+      <c r="BE249" t="n">
+        <v>953.8</v>
+      </c>
+      <c r="BF249" t="n">
+        <v>677.98</v>
+      </c>
+      <c r="BG249" t="n">
+        <v>464.45</v>
+      </c>
+      <c r="BH249" t="n">
+        <v>342.5</v>
+      </c>
+      <c r="BI249" t="n">
+        <v>50.06</v>
+      </c>
       <c r="BJ249" t="inlineStr"/>
       <c r="BK249" t="inlineStr"/>
       <c r="BL249" t="inlineStr"/>
@@ -37578,10 +38412,18 @@
       <c r="CJ249" t="inlineStr"/>
       <c r="CK249" t="inlineStr"/>
       <c r="CL249" t="inlineStr"/>
-      <c r="CM249" t="inlineStr"/>
-      <c r="CN249" t="inlineStr"/>
-      <c r="CO249" t="inlineStr"/>
-      <c r="CP249" t="inlineStr"/>
+      <c r="CM249" t="n">
+        <v>79.13</v>
+      </c>
+      <c r="CN249" t="n">
+        <v>78.37</v>
+      </c>
+      <c r="CO249" t="n">
+        <v>148.47</v>
+      </c>
+      <c r="CP249" t="n">
+        <v>365.7</v>
+      </c>
     </row>
     <row r="250">
       <c r="A250" t="n">
@@ -37837,14 +38679,30 @@
       <c r="BA251" t="n">
         <v>2008</v>
       </c>
-      <c r="BB251" t="inlineStr"/>
-      <c r="BC251" t="inlineStr"/>
-      <c r="BD251" t="inlineStr"/>
-      <c r="BE251" t="inlineStr"/>
-      <c r="BF251" t="inlineStr"/>
-      <c r="BG251" t="inlineStr"/>
-      <c r="BH251" t="inlineStr"/>
-      <c r="BI251" t="inlineStr"/>
+      <c r="BB251" t="n">
+        <v>2946.44</v>
+      </c>
+      <c r="BC251" t="n">
+        <v>2747.86</v>
+      </c>
+      <c r="BD251" t="n">
+        <v>2705</v>
+      </c>
+      <c r="BE251" t="n">
+        <v>3139.8</v>
+      </c>
+      <c r="BF251" t="n">
+        <v>3233.78</v>
+      </c>
+      <c r="BG251" t="n">
+        <v>3233.45</v>
+      </c>
+      <c r="BH251" t="n">
+        <v>3232.41</v>
+      </c>
+      <c r="BI251" t="n">
+        <v>3288.72</v>
+      </c>
       <c r="BJ251" t="inlineStr"/>
       <c r="BK251" t="inlineStr"/>
       <c r="BL251" t="inlineStr"/>
@@ -37874,10 +38732,18 @@
       <c r="CJ251" t="inlineStr"/>
       <c r="CK251" t="inlineStr"/>
       <c r="CL251" t="inlineStr"/>
-      <c r="CM251" t="inlineStr"/>
-      <c r="CN251" t="inlineStr"/>
-      <c r="CO251" t="inlineStr"/>
-      <c r="CP251" t="inlineStr"/>
+      <c r="CM251" t="n">
+        <v>3245.11</v>
+      </c>
+      <c r="CN251" t="n">
+        <v>3136.1</v>
+      </c>
+      <c r="CO251" t="n">
+        <v>3441.98</v>
+      </c>
+      <c r="CP251" t="n">
+        <v>2984.12</v>
+      </c>
     </row>
     <row r="252">
       <c r="A252" t="n">
@@ -37983,12 +38849,24 @@
       <c r="BA252" t="n">
         <v>2008</v>
       </c>
-      <c r="BB252" t="inlineStr"/>
-      <c r="BC252" t="inlineStr"/>
-      <c r="BD252" t="inlineStr"/>
-      <c r="BE252" t="inlineStr"/>
-      <c r="BF252" t="inlineStr"/>
-      <c r="BG252" t="inlineStr"/>
+      <c r="BB252" t="n">
+        <v>5016.63</v>
+      </c>
+      <c r="BC252" t="n">
+        <v>108.53</v>
+      </c>
+      <c r="BD252" t="n">
+        <v>148.96</v>
+      </c>
+      <c r="BE252" t="n">
+        <v>83.06</v>
+      </c>
+      <c r="BF252" t="n">
+        <v>81.22</v>
+      </c>
+      <c r="BG252" t="n">
+        <v>85.47</v>
+      </c>
       <c r="BH252" t="inlineStr"/>
       <c r="BI252" t="inlineStr"/>
       <c r="BJ252" t="inlineStr"/>
@@ -38020,10 +38898,18 @@
       <c r="CJ252" t="inlineStr"/>
       <c r="CK252" t="inlineStr"/>
       <c r="CL252" t="inlineStr"/>
-      <c r="CM252" t="inlineStr"/>
-      <c r="CN252" t="inlineStr"/>
-      <c r="CO252" t="inlineStr"/>
-      <c r="CP252" t="inlineStr"/>
+      <c r="CM252" t="n">
+        <v>75.92</v>
+      </c>
+      <c r="CN252" t="n">
+        <v>102.93</v>
+      </c>
+      <c r="CO252" t="n">
+        <v>117.44</v>
+      </c>
+      <c r="CP252" t="n">
+        <v>44.15</v>
+      </c>
     </row>
     <row r="253">
       <c r="A253" t="n">
@@ -38129,12 +39015,24 @@
       <c r="BA253" t="n">
         <v>2008</v>
       </c>
-      <c r="BB253" t="inlineStr"/>
-      <c r="BC253" t="inlineStr"/>
-      <c r="BD253" t="inlineStr"/>
-      <c r="BE253" t="inlineStr"/>
-      <c r="BF253" t="inlineStr"/>
-      <c r="BG253" t="inlineStr"/>
+      <c r="BB253" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC253" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD253" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE253" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF253" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG253" t="n">
+        <v>3972.97</v>
+      </c>
       <c r="BH253" t="inlineStr"/>
       <c r="BI253" t="inlineStr"/>
       <c r="BJ253" t="inlineStr"/>
@@ -38166,10 +39064,18 @@
       <c r="CJ253" t="inlineStr"/>
       <c r="CK253" t="inlineStr"/>
       <c r="CL253" t="inlineStr"/>
-      <c r="CM253" t="inlineStr"/>
-      <c r="CN253" t="inlineStr"/>
-      <c r="CO253" t="inlineStr"/>
-      <c r="CP253" t="inlineStr"/>
+      <c r="CM253" t="n">
+        <v>2516.92</v>
+      </c>
+      <c r="CN253" t="n">
+        <v>2516.93</v>
+      </c>
+      <c r="CO253" t="n">
+        <v>1833.72</v>
+      </c>
+      <c r="CP253" t="n">
+        <v>1611.41</v>
+      </c>
     </row>
     <row r="254">
       <c r="A254" t="n">
@@ -38275,12 +39181,24 @@
       <c r="BA254" t="n">
         <v>2008</v>
       </c>
-      <c r="BB254" t="inlineStr"/>
-      <c r="BC254" t="inlineStr"/>
-      <c r="BD254" t="inlineStr"/>
-      <c r="BE254" t="inlineStr"/>
-      <c r="BF254" t="inlineStr"/>
-      <c r="BG254" t="inlineStr"/>
+      <c r="BB254" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC254" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD254" t="n">
+        <v>1163.7</v>
+      </c>
+      <c r="BE254" t="n">
+        <v>801.17</v>
+      </c>
+      <c r="BF254" t="n">
+        <v>309.06</v>
+      </c>
+      <c r="BG254" t="n">
+        <v>222.31</v>
+      </c>
       <c r="BH254" t="inlineStr"/>
       <c r="BI254" t="inlineStr"/>
       <c r="BJ254" t="inlineStr"/>
@@ -38312,10 +39230,18 @@
       <c r="CJ254" t="inlineStr"/>
       <c r="CK254" t="inlineStr"/>
       <c r="CL254" t="inlineStr"/>
-      <c r="CM254" t="inlineStr"/>
-      <c r="CN254" t="inlineStr"/>
-      <c r="CO254" t="inlineStr"/>
-      <c r="CP254" t="inlineStr"/>
+      <c r="CM254" t="n">
+        <v>226.14</v>
+      </c>
+      <c r="CN254" t="n">
+        <v>161.22</v>
+      </c>
+      <c r="CO254" t="n">
+        <v>117.24</v>
+      </c>
+      <c r="CP254" t="n">
+        <v>104.13</v>
+      </c>
     </row>
     <row r="255">
       <c r="A255" t="n">
@@ -38421,12 +39347,24 @@
       <c r="BA255" t="n">
         <v>2008</v>
       </c>
-      <c r="BB255" t="inlineStr"/>
-      <c r="BC255" t="inlineStr"/>
-      <c r="BD255" t="inlineStr"/>
-      <c r="BE255" t="inlineStr"/>
-      <c r="BF255" t="inlineStr"/>
-      <c r="BG255" t="inlineStr"/>
+      <c r="BB255" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC255" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD255" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE255" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF255" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG255" t="n">
+        <v>0</v>
+      </c>
       <c r="BH255" t="inlineStr"/>
       <c r="BI255" t="inlineStr"/>
       <c r="BJ255" t="inlineStr"/>
@@ -38458,10 +39396,18 @@
       <c r="CJ255" t="inlineStr"/>
       <c r="CK255" t="inlineStr"/>
       <c r="CL255" t="inlineStr"/>
-      <c r="CM255" t="inlineStr"/>
-      <c r="CN255" t="inlineStr"/>
-      <c r="CO255" t="inlineStr"/>
-      <c r="CP255" t="inlineStr"/>
+      <c r="CM255" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN255" t="n">
+        <v>144.48</v>
+      </c>
+      <c r="CO255" t="n">
+        <v>168.97</v>
+      </c>
+      <c r="CP255" t="n">
+        <v>126.17</v>
+      </c>
     </row>
     <row r="256">
       <c r="A256" t="n">
@@ -38709,12 +39655,24 @@
       <c r="BA257" t="n">
         <v>2008</v>
       </c>
-      <c r="BB257" t="inlineStr"/>
-      <c r="BC257" t="inlineStr"/>
-      <c r="BD257" t="inlineStr"/>
-      <c r="BE257" t="inlineStr"/>
-      <c r="BF257" t="inlineStr"/>
-      <c r="BG257" t="inlineStr"/>
+      <c r="BB257" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC257" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD257" t="n">
+        <v>2.32</v>
+      </c>
+      <c r="BE257" t="n">
+        <v>347.57</v>
+      </c>
+      <c r="BF257" t="n">
+        <v>124.7</v>
+      </c>
+      <c r="BG257" t="n">
+        <v>86.34</v>
+      </c>
       <c r="BH257" t="inlineStr"/>
       <c r="BI257" t="inlineStr"/>
       <c r="BJ257" t="inlineStr"/>
@@ -38746,10 +39704,18 @@
       <c r="CJ257" t="inlineStr"/>
       <c r="CK257" t="inlineStr"/>
       <c r="CL257" t="inlineStr"/>
-      <c r="CM257" t="inlineStr"/>
-      <c r="CN257" t="inlineStr"/>
-      <c r="CO257" t="inlineStr"/>
-      <c r="CP257" t="inlineStr"/>
+      <c r="CM257" t="n">
+        <v>115.38</v>
+      </c>
+      <c r="CN257" t="n">
+        <v>120.06</v>
+      </c>
+      <c r="CO257" t="n">
+        <v>112.41</v>
+      </c>
+      <c r="CP257" t="n">
+        <v>96.59999999999999</v>
+      </c>
     </row>
     <row r="258">
       <c r="A258" t="n">
@@ -39575,9 +40541,15 @@
       <c r="BG262" t="inlineStr"/>
       <c r="BH262" t="inlineStr"/>
       <c r="BI262" t="inlineStr"/>
-      <c r="BJ262" t="inlineStr"/>
-      <c r="BK262" t="inlineStr"/>
-      <c r="BL262" t="inlineStr"/>
+      <c r="BJ262" t="n">
+        <v>89.28</v>
+      </c>
+      <c r="BK262" t="n">
+        <v>95.84</v>
+      </c>
+      <c r="BL262" t="n">
+        <v>85.98</v>
+      </c>
       <c r="BM262" t="inlineStr"/>
       <c r="BN262" t="inlineStr"/>
       <c r="BO262" t="inlineStr"/>
@@ -39604,10 +40576,18 @@
       <c r="CJ262" t="inlineStr"/>
       <c r="CK262" t="inlineStr"/>
       <c r="CL262" t="inlineStr"/>
-      <c r="CM262" t="inlineStr"/>
-      <c r="CN262" t="inlineStr"/>
-      <c r="CO262" t="inlineStr"/>
-      <c r="CP262" t="inlineStr"/>
+      <c r="CM262" t="n">
+        <v>197.01</v>
+      </c>
+      <c r="CN262" t="n">
+        <v>205.89</v>
+      </c>
+      <c r="CO262" t="n">
+        <v>175.99</v>
+      </c>
+      <c r="CP262" t="n">
+        <v>190.2</v>
+      </c>
     </row>
     <row r="263">
       <c r="A263" t="n">
@@ -39740,9 +40720,15 @@
       <c r="BJ263" t="inlineStr"/>
       <c r="BK263" t="inlineStr"/>
       <c r="BL263" t="inlineStr"/>
-      <c r="BM263" t="inlineStr"/>
-      <c r="BN263" t="inlineStr"/>
-      <c r="BO263" t="inlineStr"/>
+      <c r="BM263" t="n">
+        <v>136.25</v>
+      </c>
+      <c r="BN263" t="n">
+        <v>131.73</v>
+      </c>
+      <c r="BO263" t="n">
+        <v>128.16</v>
+      </c>
       <c r="BP263" t="inlineStr"/>
       <c r="BQ263" t="inlineStr"/>
       <c r="BR263" t="inlineStr"/>
@@ -39766,10 +40752,18 @@
       <c r="CJ263" t="inlineStr"/>
       <c r="CK263" t="inlineStr"/>
       <c r="CL263" t="inlineStr"/>
-      <c r="CM263" t="inlineStr"/>
-      <c r="CN263" t="inlineStr"/>
-      <c r="CO263" t="inlineStr"/>
-      <c r="CP263" t="inlineStr"/>
+      <c r="CM263" t="n">
+        <v>153.64</v>
+      </c>
+      <c r="CN263" t="n">
+        <v>123.94</v>
+      </c>
+      <c r="CO263" t="n">
+        <v>86.31</v>
+      </c>
+      <c r="CP263" t="n">
+        <v>169.89</v>
+      </c>
     </row>
     <row r="264">
       <c r="A264" t="n">
@@ -39871,10 +40865,18 @@
       <c r="BA264" t="n">
         <v>2006</v>
       </c>
-      <c r="BB264" t="inlineStr"/>
-      <c r="BC264" t="inlineStr"/>
-      <c r="BD264" t="inlineStr"/>
-      <c r="BE264" t="inlineStr"/>
+      <c r="BB264" t="n">
+        <v>687.84</v>
+      </c>
+      <c r="BC264" t="n">
+        <v>414.02</v>
+      </c>
+      <c r="BD264" t="n">
+        <v>883.98</v>
+      </c>
+      <c r="BE264" t="n">
+        <v>277.19</v>
+      </c>
       <c r="BF264" t="inlineStr"/>
       <c r="BG264" t="inlineStr"/>
       <c r="BH264" t="inlineStr"/>
@@ -39908,10 +40910,18 @@
       <c r="CJ264" t="inlineStr"/>
       <c r="CK264" t="inlineStr"/>
       <c r="CL264" t="inlineStr"/>
-      <c r="CM264" t="inlineStr"/>
-      <c r="CN264" t="inlineStr"/>
-      <c r="CO264" t="inlineStr"/>
-      <c r="CP264" t="inlineStr"/>
+      <c r="CM264" t="n">
+        <v>277.19</v>
+      </c>
+      <c r="CN264" t="n">
+        <v>231.15</v>
+      </c>
+      <c r="CO264" t="n">
+        <v>227.02</v>
+      </c>
+      <c r="CP264" t="n">
+        <v>139.38</v>
+      </c>
     </row>
     <row r="265">
       <c r="A265" t="n">
@@ -40175,11 +41185,21 @@
       <c r="BC266" t="inlineStr"/>
       <c r="BD266" t="inlineStr"/>
       <c r="BE266" t="inlineStr"/>
-      <c r="BF266" t="inlineStr"/>
-      <c r="BG266" t="inlineStr"/>
-      <c r="BH266" t="inlineStr"/>
-      <c r="BI266" t="inlineStr"/>
-      <c r="BJ266" t="inlineStr"/>
+      <c r="BF266" t="n">
+        <v>62.53</v>
+      </c>
+      <c r="BG266" t="n">
+        <v>57.25</v>
+      </c>
+      <c r="BH266" t="n">
+        <v>126.46</v>
+      </c>
+      <c r="BI266" t="n">
+        <v>280.45</v>
+      </c>
+      <c r="BJ266" t="n">
+        <v>165.24</v>
+      </c>
       <c r="BK266" t="inlineStr"/>
       <c r="BL266" t="inlineStr"/>
       <c r="BM266" t="inlineStr"/>
@@ -40208,10 +41228,18 @@
       <c r="CJ266" t="inlineStr"/>
       <c r="CK266" t="inlineStr"/>
       <c r="CL266" t="inlineStr"/>
-      <c r="CM266" t="inlineStr"/>
-      <c r="CN266" t="inlineStr"/>
-      <c r="CO266" t="inlineStr"/>
-      <c r="CP266" t="inlineStr"/>
+      <c r="CM266" t="n">
+        <v>150.74</v>
+      </c>
+      <c r="CN266" t="n">
+        <v>162.87</v>
+      </c>
+      <c r="CO266" t="n">
+        <v>152.63</v>
+      </c>
+      <c r="CP266" t="n">
+        <v>139.77</v>
+      </c>
     </row>
     <row r="267">
       <c r="A267" t="n">
@@ -40327,11 +41355,21 @@
       <c r="BC267" t="inlineStr"/>
       <c r="BD267" t="inlineStr"/>
       <c r="BE267" t="inlineStr"/>
-      <c r="BF267" t="inlineStr"/>
-      <c r="BG267" t="inlineStr"/>
-      <c r="BH267" t="inlineStr"/>
-      <c r="BI267" t="inlineStr"/>
-      <c r="BJ267" t="inlineStr"/>
+      <c r="BF267" t="n">
+        <v>663.85</v>
+      </c>
+      <c r="BG267" t="n">
+        <v>341.79</v>
+      </c>
+      <c r="BH267" t="n">
+        <v>341.94</v>
+      </c>
+      <c r="BI267" t="n">
+        <v>342.01</v>
+      </c>
+      <c r="BJ267" t="n">
+        <v>1056.26</v>
+      </c>
       <c r="BK267" t="inlineStr"/>
       <c r="BL267" t="inlineStr"/>
       <c r="BM267" t="inlineStr"/>
@@ -40360,10 +41398,18 @@
       <c r="CJ267" t="inlineStr"/>
       <c r="CK267" t="inlineStr"/>
       <c r="CL267" t="inlineStr"/>
-      <c r="CM267" t="inlineStr"/>
-      <c r="CN267" t="inlineStr"/>
-      <c r="CO267" t="inlineStr"/>
-      <c r="CP267" t="inlineStr"/>
+      <c r="CM267" t="n">
+        <v>1056.47</v>
+      </c>
+      <c r="CN267" t="n">
+        <v>1251.03</v>
+      </c>
+      <c r="CO267" t="n">
+        <v>109.76</v>
+      </c>
+      <c r="CP267" t="n">
+        <v>1294.8</v>
+      </c>
     </row>
     <row r="268">
       <c r="A268" t="n">
@@ -40467,11 +41513,21 @@
       <c r="BA268" t="n">
         <v>2005</v>
       </c>
-      <c r="BB268" t="inlineStr"/>
-      <c r="BC268" t="inlineStr"/>
-      <c r="BD268" t="inlineStr"/>
-      <c r="BE268" t="inlineStr"/>
-      <c r="BF268" t="inlineStr"/>
+      <c r="BB268" t="n">
+        <v>4225.22</v>
+      </c>
+      <c r="BC268" t="n">
+        <v>3983.75</v>
+      </c>
+      <c r="BD268" t="n">
+        <v>4008.82</v>
+      </c>
+      <c r="BE268" t="n">
+        <v>4027.78</v>
+      </c>
+      <c r="BF268" t="n">
+        <v>4008.03</v>
+      </c>
       <c r="BG268" t="inlineStr"/>
       <c r="BH268" t="inlineStr"/>
       <c r="BI268" t="inlineStr"/>
@@ -40504,10 +41560,18 @@
       <c r="CJ268" t="inlineStr"/>
       <c r="CK268" t="inlineStr"/>
       <c r="CL268" t="inlineStr"/>
-      <c r="CM268" t="inlineStr"/>
-      <c r="CN268" t="inlineStr"/>
-      <c r="CO268" t="inlineStr"/>
-      <c r="CP268" t="inlineStr"/>
+      <c r="CM268" t="n">
+        <v>7.18</v>
+      </c>
+      <c r="CN268" t="n">
+        <v>3973.15</v>
+      </c>
+      <c r="CO268" t="n">
+        <v>3972.35</v>
+      </c>
+      <c r="CP268" t="n">
+        <v>4023.12</v>
+      </c>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
@@ -40777,10 +41841,18 @@
       <c r="BA270" t="n">
         <v>2003</v>
       </c>
-      <c r="BB270" t="inlineStr"/>
-      <c r="BC270" t="inlineStr"/>
-      <c r="BD270" t="inlineStr"/>
-      <c r="BE270" t="inlineStr"/>
+      <c r="BB270" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC270" t="n">
+        <v>264.81</v>
+      </c>
+      <c r="BD270" t="n">
+        <v>916409.73</v>
+      </c>
+      <c r="BE270" t="n">
+        <v>162045.59</v>
+      </c>
       <c r="BF270" t="inlineStr"/>
       <c r="BG270" t="inlineStr"/>
       <c r="BH270" t="inlineStr"/>
@@ -40814,10 +41886,18 @@
       <c r="CJ270" t="inlineStr"/>
       <c r="CK270" t="inlineStr"/>
       <c r="CL270" t="inlineStr"/>
-      <c r="CM270" t="inlineStr"/>
-      <c r="CN270" t="inlineStr"/>
-      <c r="CO270" t="inlineStr"/>
-      <c r="CP270" t="inlineStr"/>
+      <c r="CM270" t="n">
+        <v>162045.59</v>
+      </c>
+      <c r="CN270" t="n">
+        <v>40.04</v>
+      </c>
+      <c r="CO270" t="n">
+        <v>63.64</v>
+      </c>
+      <c r="CP270" t="n">
+        <v>9301.01</v>
+      </c>
     </row>
     <row r="271">
       <c r="A271" t="n">
@@ -41203,13 +42283,27 @@
       <c r="BA273" t="n">
         <v>2008</v>
       </c>
-      <c r="BB273" t="inlineStr"/>
-      <c r="BC273" t="inlineStr"/>
-      <c r="BD273" t="inlineStr"/>
-      <c r="BE273" t="inlineStr"/>
-      <c r="BF273" t="inlineStr"/>
-      <c r="BG273" t="inlineStr"/>
-      <c r="BH273" t="inlineStr"/>
+      <c r="BB273" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC273" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD273" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE273" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF273" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG273" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH273" t="n">
+        <v>0</v>
+      </c>
       <c r="BI273" t="inlineStr"/>
       <c r="BJ273" t="inlineStr"/>
       <c r="BK273" t="inlineStr"/>
@@ -41240,10 +42334,18 @@
       <c r="CJ273" t="inlineStr"/>
       <c r="CK273" t="inlineStr"/>
       <c r="CL273" t="inlineStr"/>
-      <c r="CM273" t="inlineStr"/>
-      <c r="CN273" t="inlineStr"/>
-      <c r="CO273" t="inlineStr"/>
-      <c r="CP273" t="inlineStr"/>
+      <c r="CM273" t="n">
+        <v>6437.72</v>
+      </c>
+      <c r="CN273" t="n">
+        <v>6437.58</v>
+      </c>
+      <c r="CO273" t="n">
+        <v>6372.86</v>
+      </c>
+      <c r="CP273" t="n">
+        <v>1314.5</v>
+      </c>
     </row>
     <row r="274">
       <c r="A274" t="n">
@@ -42385,11 +43487,21 @@
       <c r="BA280" t="n">
         <v>2007</v>
       </c>
-      <c r="BB280" t="inlineStr"/>
-      <c r="BC280" t="inlineStr"/>
-      <c r="BD280" t="inlineStr"/>
-      <c r="BE280" t="inlineStr"/>
-      <c r="BF280" t="inlineStr"/>
+      <c r="BB280" t="n">
+        <v>2596.84</v>
+      </c>
+      <c r="BC280" t="n">
+        <v>2573.26</v>
+      </c>
+      <c r="BD280" t="n">
+        <v>2707.18</v>
+      </c>
+      <c r="BE280" t="n">
+        <v>2709.42</v>
+      </c>
+      <c r="BF280" t="n">
+        <v>2654.34</v>
+      </c>
       <c r="BG280" t="inlineStr"/>
       <c r="BH280" t="inlineStr"/>
       <c r="BI280" t="inlineStr"/>
@@ -42422,10 +43534,18 @@
       <c r="CJ280" t="inlineStr"/>
       <c r="CK280" t="inlineStr"/>
       <c r="CL280" t="inlineStr"/>
-      <c r="CM280" t="inlineStr"/>
-      <c r="CN280" t="inlineStr"/>
-      <c r="CO280" t="inlineStr"/>
-      <c r="CP280" t="inlineStr"/>
+      <c r="CM280" t="n">
+        <v>2704.86</v>
+      </c>
+      <c r="CN280" t="n">
+        <v>2704.89</v>
+      </c>
+      <c r="CO280" t="n">
+        <v>2689.91</v>
+      </c>
+      <c r="CP280" t="n">
+        <v>2690.79</v>
+      </c>
     </row>
     <row r="281">
       <c r="A281" t="n">
@@ -42529,11 +43649,21 @@
       <c r="BA281" t="n">
         <v>2007</v>
       </c>
-      <c r="BB281" t="inlineStr"/>
-      <c r="BC281" t="inlineStr"/>
-      <c r="BD281" t="inlineStr"/>
-      <c r="BE281" t="inlineStr"/>
-      <c r="BF281" t="inlineStr"/>
+      <c r="BB281" t="n">
+        <v>93.66</v>
+      </c>
+      <c r="BC281" t="n">
+        <v>78.51000000000001</v>
+      </c>
+      <c r="BD281" t="n">
+        <v>74.7</v>
+      </c>
+      <c r="BE281" t="n">
+        <v>75.09</v>
+      </c>
+      <c r="BF281" t="n">
+        <v>78.34</v>
+      </c>
       <c r="BG281" t="inlineStr"/>
       <c r="BH281" t="inlineStr"/>
       <c r="BI281" t="inlineStr"/>
@@ -42566,10 +43696,18 @@
       <c r="CJ281" t="inlineStr"/>
       <c r="CK281" t="inlineStr"/>
       <c r="CL281" t="inlineStr"/>
-      <c r="CM281" t="inlineStr"/>
-      <c r="CN281" t="inlineStr"/>
-      <c r="CO281" t="inlineStr"/>
-      <c r="CP281" t="inlineStr"/>
+      <c r="CM281" t="n">
+        <v>74.40000000000001</v>
+      </c>
+      <c r="CN281" t="n">
+        <v>66.73999999999999</v>
+      </c>
+      <c r="CO281" t="n">
+        <v>63.28</v>
+      </c>
+      <c r="CP281" t="n">
+        <v>54.01</v>
+      </c>
     </row>
     <row r="282">
       <c r="A282" t="n">
@@ -42673,11 +43811,21 @@
       <c r="BA282" t="n">
         <v>2007</v>
       </c>
-      <c r="BB282" t="inlineStr"/>
-      <c r="BC282" t="inlineStr"/>
-      <c r="BD282" t="inlineStr"/>
-      <c r="BE282" t="inlineStr"/>
-      <c r="BF282" t="inlineStr"/>
+      <c r="BB282" t="n">
+        <v>92.11</v>
+      </c>
+      <c r="BC282" t="n">
+        <v>104.6</v>
+      </c>
+      <c r="BD282" t="n">
+        <v>101.37</v>
+      </c>
+      <c r="BE282" t="n">
+        <v>116.58</v>
+      </c>
+      <c r="BF282" t="n">
+        <v>108.66</v>
+      </c>
       <c r="BG282" t="inlineStr"/>
       <c r="BH282" t="inlineStr"/>
       <c r="BI282" t="inlineStr"/>
@@ -42710,10 +43858,18 @@
       <c r="CJ282" t="inlineStr"/>
       <c r="CK282" t="inlineStr"/>
       <c r="CL282" t="inlineStr"/>
-      <c r="CM282" t="inlineStr"/>
-      <c r="CN282" t="inlineStr"/>
-      <c r="CO282" t="inlineStr"/>
-      <c r="CP282" t="inlineStr"/>
+      <c r="CM282" t="n">
+        <v>149.84</v>
+      </c>
+      <c r="CN282" t="n">
+        <v>122.21</v>
+      </c>
+      <c r="CO282" t="n">
+        <v>116.99</v>
+      </c>
+      <c r="CP282" t="n">
+        <v>110.29</v>
+      </c>
     </row>
     <row r="283">
       <c r="A283" t="n">
@@ -42817,11 +43973,21 @@
       <c r="BA283" t="n">
         <v>2007</v>
       </c>
-      <c r="BB283" t="inlineStr"/>
-      <c r="BC283" t="inlineStr"/>
-      <c r="BD283" t="inlineStr"/>
-      <c r="BE283" t="inlineStr"/>
-      <c r="BF283" t="inlineStr"/>
+      <c r="BB283" t="n">
+        <v>4.73</v>
+      </c>
+      <c r="BC283" t="n">
+        <v>4.68</v>
+      </c>
+      <c r="BD283" t="n">
+        <v>5.18</v>
+      </c>
+      <c r="BE283" t="n">
+        <v>6.43</v>
+      </c>
+      <c r="BF283" t="n">
+        <v>64.58</v>
+      </c>
       <c r="BG283" t="inlineStr"/>
       <c r="BH283" t="inlineStr"/>
       <c r="BI283" t="inlineStr"/>
@@ -42854,10 +44020,18 @@
       <c r="CJ283" t="inlineStr"/>
       <c r="CK283" t="inlineStr"/>
       <c r="CL283" t="inlineStr"/>
-      <c r="CM283" t="inlineStr"/>
-      <c r="CN283" t="inlineStr"/>
-      <c r="CO283" t="inlineStr"/>
-      <c r="CP283" t="inlineStr"/>
+      <c r="CM283" t="n">
+        <v>28.06</v>
+      </c>
+      <c r="CN283" t="n">
+        <v>62.66</v>
+      </c>
+      <c r="CO283" t="n">
+        <v>2.24</v>
+      </c>
+      <c r="CP283" t="n">
+        <v>2.24</v>
+      </c>
     </row>
     <row r="284">
       <c r="A284" t="n">
@@ -43528,13 +44702,27 @@
         <v>2007</v>
       </c>
       <c r="BB288" t="inlineStr"/>
-      <c r="BC288" t="inlineStr"/>
-      <c r="BD288" t="inlineStr"/>
-      <c r="BE288" t="inlineStr"/>
-      <c r="BF288" t="inlineStr"/>
-      <c r="BG288" t="inlineStr"/>
-      <c r="BH288" t="inlineStr"/>
-      <c r="BI288" t="inlineStr"/>
+      <c r="BC288" t="n">
+        <v>1827.28</v>
+      </c>
+      <c r="BD288" t="n">
+        <v>1827.24</v>
+      </c>
+      <c r="BE288" t="n">
+        <v>1812.3</v>
+      </c>
+      <c r="BF288" t="n">
+        <v>1337.52</v>
+      </c>
+      <c r="BG288" t="n">
+        <v>257.01</v>
+      </c>
+      <c r="BH288" t="n">
+        <v>257.91</v>
+      </c>
+      <c r="BI288" t="n">
+        <v>54.62</v>
+      </c>
       <c r="BJ288" t="inlineStr"/>
       <c r="BK288" t="inlineStr"/>
       <c r="BL288" t="inlineStr"/>
@@ -43564,10 +44752,18 @@
       <c r="CJ288" t="inlineStr"/>
       <c r="CK288" t="inlineStr"/>
       <c r="CL288" t="inlineStr"/>
-      <c r="CM288" t="inlineStr"/>
-      <c r="CN288" t="inlineStr"/>
-      <c r="CO288" t="inlineStr"/>
-      <c r="CP288" t="inlineStr"/>
+      <c r="CM288" t="n">
+        <v>87.06999999999999</v>
+      </c>
+      <c r="CN288" t="n">
+        <v>252.7</v>
+      </c>
+      <c r="CO288" t="n">
+        <v>792.52</v>
+      </c>
+      <c r="CP288" t="n">
+        <v>305.39</v>
+      </c>
     </row>
     <row r="289">
       <c r="A289" t="n">
@@ -43963,12 +45159,24 @@
       <c r="BA291" t="n">
         <v>2010</v>
       </c>
-      <c r="BB291" t="inlineStr"/>
-      <c r="BC291" t="inlineStr"/>
-      <c r="BD291" t="inlineStr"/>
-      <c r="BE291" t="inlineStr"/>
-      <c r="BF291" t="inlineStr"/>
-      <c r="BG291" t="inlineStr"/>
+      <c r="BB291" t="n">
+        <v>429.39</v>
+      </c>
+      <c r="BC291" t="n">
+        <v>509.97</v>
+      </c>
+      <c r="BD291" t="n">
+        <v>555.53</v>
+      </c>
+      <c r="BE291" t="n">
+        <v>580.92</v>
+      </c>
+      <c r="BF291" t="n">
+        <v>451.26</v>
+      </c>
+      <c r="BG291" t="n">
+        <v>561.66</v>
+      </c>
       <c r="BH291" t="inlineStr"/>
       <c r="BI291" t="inlineStr"/>
       <c r="BJ291" t="inlineStr"/>
@@ -44000,10 +45208,18 @@
       <c r="CJ291" t="inlineStr"/>
       <c r="CK291" t="inlineStr"/>
       <c r="CL291" t="inlineStr"/>
-      <c r="CM291" t="inlineStr"/>
-      <c r="CN291" t="inlineStr"/>
-      <c r="CO291" t="inlineStr"/>
-      <c r="CP291" t="inlineStr"/>
+      <c r="CM291" t="n">
+        <v>502.52</v>
+      </c>
+      <c r="CN291" t="n">
+        <v>548.33</v>
+      </c>
+      <c r="CO291" t="n">
+        <v>492.47</v>
+      </c>
+      <c r="CP291" t="n">
+        <v>418.12</v>
+      </c>
     </row>
     <row r="292">
       <c r="A292" t="n">
@@ -44109,12 +45325,24 @@
       <c r="BA292" t="n">
         <v>2010</v>
       </c>
-      <c r="BB292" t="inlineStr"/>
-      <c r="BC292" t="inlineStr"/>
-      <c r="BD292" t="inlineStr"/>
-      <c r="BE292" t="inlineStr"/>
-      <c r="BF292" t="inlineStr"/>
-      <c r="BG292" t="inlineStr"/>
+      <c r="BB292" t="n">
+        <v>79.16</v>
+      </c>
+      <c r="BC292" t="n">
+        <v>62.55</v>
+      </c>
+      <c r="BD292" t="n">
+        <v>32.97</v>
+      </c>
+      <c r="BE292" t="n">
+        <v>28.61</v>
+      </c>
+      <c r="BF292" t="n">
+        <v>26.83</v>
+      </c>
+      <c r="BG292" t="n">
+        <v>23.34</v>
+      </c>
       <c r="BH292" t="inlineStr"/>
       <c r="BI292" t="inlineStr"/>
       <c r="BJ292" t="inlineStr"/>
@@ -44146,10 +45374,18 @@
       <c r="CJ292" t="inlineStr"/>
       <c r="CK292" t="inlineStr"/>
       <c r="CL292" t="inlineStr"/>
-      <c r="CM292" t="inlineStr"/>
-      <c r="CN292" t="inlineStr"/>
-      <c r="CO292" t="inlineStr"/>
-      <c r="CP292" t="inlineStr"/>
+      <c r="CM292" t="n">
+        <v>42.84</v>
+      </c>
+      <c r="CN292" t="n">
+        <v>39.58</v>
+      </c>
+      <c r="CO292" t="n">
+        <v>38.05</v>
+      </c>
+      <c r="CP292" t="n">
+        <v>39.48</v>
+      </c>
     </row>
     <row r="293">
       <c r="A293" t="n">

</xml_diff>